<commit_message>
Story 5:Create Cooler requirement and Traceability Matrix
</commit_message>
<xml_diff>
--- a/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
+++ b/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
@@ -359,12 +359,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -407,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -447,15 +453,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1164,7 +1171,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1183,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
+      <c r="A1" s="18"/>
       <c r="B1" s="7" t="s">
         <v>72</v>
       </c>
@@ -1207,7 +1214,7 @@
       <c r="K1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="17" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1215,7 +1222,7 @@
       <c r="A2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
@@ -1225,20 +1232,20 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="15"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>93</v>
       </c>
       <c r="F3" s="14"/>
@@ -1247,7 +1254,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1259,25 +1266,25 @@
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1286,24 +1293,24 @@
         <v>67</v>
       </c>
       <c r="B5" s="14"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>93</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Story 9:Made and changed Cooler Traceability Matrix
</commit_message>
<xml_diff>
--- a/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
+++ b/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Требования к кулеру" sheetId="1" r:id="rId1"/>
-    <sheet name="формулировка требований" sheetId="5" r:id="rId2"/>
-    <sheet name="проверка" sheetId="6" r:id="rId3"/>
-    <sheet name="Traceability matrix" sheetId="4" r:id="rId4"/>
+    <sheet name="BRD" sheetId="5" r:id="rId2"/>
+    <sheet name="FRD" sheetId="6" r:id="rId3"/>
+    <sheet name="Test scenarios" sheetId="4" r:id="rId4"/>
+    <sheet name="Traceability Matrix" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="167">
   <si>
     <t>Правильность</t>
   </si>
@@ -216,101 +217,320 @@
     <t>"PLUS" Кулер для воды должен быть прямоугольной формы, выполнен по ГОСТу. Должен иметь отсек для хранение посуды, холодильную камеру, четыре посуды.</t>
   </si>
   <si>
-    <t>ID требования</t>
-  </si>
-  <si>
-    <t>Rq1</t>
-  </si>
-  <si>
-    <t>Rq2</t>
-  </si>
-  <si>
-    <t>Rq3</t>
-  </si>
-  <si>
-    <t>Формулировка требований:</t>
-  </si>
-  <si>
-    <t>Кулер для воды должен иметь капельный лоток, отсек для хранения и озонирывания стаканов, обьем стакана 0,33 литов. Отсек для хранения должен быть  реализован согласно ГОСТу, материал пластик, обьем вмещаемости 5 кубических метров. Отскек хранения стаканов должен иметь озонатор.</t>
-  </si>
-  <si>
-    <t>Должен реализовывать функцию подачи воды. Вода должна быть охложденная до температуры между 5 и 10 градусов за Цельсием, подогрев до температуры 90 градусов за Цельсием, очищеная и газированая. Функция охлождения должна быть реализована компресором мощностью 80 Вт.</t>
-  </si>
-  <si>
-    <t>Должен иметь холодильную камеру. Она должна быть расположеная в нижней части кулера для воды. Должна иметь обьем 20 кубических метров, прямоугольной формы, температура охлождения минус 10 градусов за Цельсием.</t>
-  </si>
-  <si>
-    <t>ID тест</t>
-  </si>
-  <si>
-    <t>Проверка</t>
-  </si>
-  <si>
-    <t>Th 1</t>
-  </si>
-  <si>
-    <t>Th2</t>
-  </si>
-  <si>
-    <t>Th 3</t>
-  </si>
-  <si>
-    <t>Выполнить визуальный осмотр на наличие ассиметрии стен, осмотр на наличие трещин и отколов.</t>
-  </si>
-  <si>
-    <t>Наполнить вместимость.</t>
-  </si>
-  <si>
-    <t>Наполнение н-го количества стаканов на деформацию.</t>
-  </si>
-  <si>
-    <t>Включение и выключение.</t>
-  </si>
-  <si>
-    <t>Измерение температуры при охлождении.</t>
-  </si>
-  <si>
-    <t>Измерение температуры при нагреве.</t>
-  </si>
-  <si>
-    <t>Взять пробу воды после очистки и сравнить.</t>
-  </si>
-  <si>
-    <t>Измерить количество газов в воде.</t>
-  </si>
-  <si>
-    <t>Измерить потребление электричества компресором.</t>
-  </si>
-  <si>
-    <t>Th 4</t>
-  </si>
-  <si>
-    <t>Th 5</t>
-  </si>
-  <si>
-    <t>Th 6</t>
-  </si>
-  <si>
-    <t>Th 7</t>
-  </si>
-  <si>
-    <t>Th 8</t>
-  </si>
-  <si>
-    <t>Th 9</t>
-  </si>
-  <si>
-    <t>Количество тестов, которые покрывают требования</t>
-  </si>
-  <si>
-    <t>+</t>
+    <t>Business requirement document:</t>
+  </si>
+  <si>
+    <t>1. Малогаборитность</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кулер для воды должен иметь прямоугольную форму с со светлыми цветами, был востребователен как в офисном помещении, так и в домашних условиях. </t>
+  </si>
+  <si>
+    <t>2. Функциональность</t>
+  </si>
+  <si>
+    <t>Кулер для воды должен иметь холодную и гарячую воду.</t>
+  </si>
+  <si>
+    <t>Также вода должа выполнять минирализацию и газирование воды.</t>
+  </si>
+  <si>
+    <t>Должен иметь отсек для хранение посуды и холодильную камеру.</t>
+  </si>
+  <si>
+    <t>3 Доступность</t>
+  </si>
+  <si>
+    <t>Кулер для воды должен иметь панель управление и маркировка краников соответственной температуры воды.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional Specification Document: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 Размерность </t>
+  </si>
+  <si>
+    <t>Кулер для воды должен иметь капельный лоток, отсек для хранения и озонирывания стаканов. Отсек для хранения должен быть  реализован согласно ГОСТу, материал пластик, обьем вмещаемости 5 кубических метров. Отскек хранения стаканов должен иметь озонатор.</t>
+  </si>
+  <si>
+    <t>Кулер для воды должен иметь холодильную камеру. Она должна быть расположеная в нижней части кулера для воды. Должна иметь обьем 20 кубических метров, прямоугольной формы.</t>
+  </si>
+  <si>
+    <t>Кулер для воды должен быть прямоугольной формы, иметь металические опоры с резиновым покрытием. Верхняя часть кулера для воды должена иметь отверствие для подачи воды вертикально в резервуар, два крана для выхода воды расположеных по центру паралельно друг другу.</t>
+  </si>
+  <si>
+    <t>Должен реализовать выдачу холодной воды с температурой между 5 и 10 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1 Функция охлождение </t>
+  </si>
+  <si>
+    <t>Должен реализовывать холод в холодильной камере, температура охлождения минус 10 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t>2.2 Функция подогрева</t>
+  </si>
+  <si>
+    <t>Должен реализовывать подачу гарячей водытемпература подогрева  должа быть 90 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t>2.3 Функция фильтрации воды</t>
+  </si>
+  <si>
+    <t>Должен осуществлять фильтрацию воды при подаче потребителю.</t>
+  </si>
+  <si>
+    <t>2.4 Функция газации фоды</t>
+  </si>
+  <si>
+    <t>Должен осуществлять функцию газирование воды.</t>
+  </si>
+  <si>
+    <t>1.2 Комплектность</t>
+  </si>
+  <si>
+    <t>Панель управления должна реализовывать подогрев и охлождение воды. При включении кулера пользователь мог выбрать температуру воды нажатием на соответствующий button. На панели управления должна быть система индикации, подсветка "синиго" цвета указывает на температуру воды от 5 до 10 градусов Цельсия, подсветка "красного" - на температур воды 90 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t>Test Objective/Test scenarios</t>
+  </si>
+  <si>
+    <t>Проверить спецификацию и чертежи устройства</t>
+  </si>
+  <si>
+    <t>Проверить сборку и разборку</t>
+  </si>
+  <si>
+    <t>Проверить целостность каждой детали</t>
+  </si>
+  <si>
+    <t>Сделать визуальный осмотр</t>
+  </si>
+  <si>
+    <t>Проверить устойчивость кулера на ровной и сухой поверхности</t>
+  </si>
+  <si>
+    <t>Проверить прочность материала корпуса устройства</t>
+  </si>
+  <si>
+    <t>Проверить подходит ли 10 литровая бутылка с водой.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить шнур питания. </t>
+  </si>
+  <si>
+    <t>Проверить вилку от шнура питания.</t>
+  </si>
+  <si>
+    <t>Проверить наличие кранов в кулере</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить расположение кранов </t>
+  </si>
+  <si>
+    <t>Проверить расположение капельный лоток</t>
+  </si>
+  <si>
+    <t>Проверить растояние между краном и капельным лотком</t>
+  </si>
+  <si>
+    <t>Проверить вмещаемость капельного лотка на количество стаканов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </t>
+  </si>
+  <si>
+    <t>Проверит отсек для хранение на вмещаемость</t>
+  </si>
+  <si>
+    <t>Проверить время затраченого на озонирование посуды</t>
+  </si>
+  <si>
+    <t>Проверить наличее холодильной камеры</t>
+  </si>
+  <si>
+    <t>Проверить плотно ли закрываеться дверь от холодильной камеры</t>
+  </si>
+  <si>
+    <t>Проверить вмещаемость холодильной камеры</t>
+  </si>
+  <si>
+    <t>Проверить выдачу воды из крана</t>
+  </si>
+  <si>
+    <t>Проверить функциональность выдачи воды из крана</t>
+  </si>
+  <si>
+    <t>Проверить температуру воды до охлождения и после</t>
+  </si>
+  <si>
+    <t>Проверить время затраченое на охлождение воды до температуры указаной заказчиком</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Провирить температуру холодильной камеры до включение и после </t>
+  </si>
+  <si>
+    <t>Проверить функциональность подачи подогретой воды</t>
+  </si>
+  <si>
+    <t>Проверить температуру воды до подогрева и после</t>
+  </si>
+  <si>
+    <t>Проверить время затраченое на подогрев воды до температуры указаной заказчиком</t>
+  </si>
+  <si>
+    <t>Проверить функциональность фильтрации воды из крана</t>
+  </si>
+  <si>
+    <t>Проверить воду на очистку до фильтрации и после.</t>
+  </si>
+  <si>
+    <t>Проверить функциональность подачи газа в воду</t>
+  </si>
+  <si>
+    <t>Проверить воду до газирования и после</t>
+  </si>
+  <si>
+    <t>Проверить наличие панели управления</t>
+  </si>
+  <si>
+    <t>Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</t>
+  </si>
+  <si>
+    <t>Проверить соответсвие кнопок функционированию</t>
+  </si>
+  <si>
+    <t>Проверить расположение панели управления</t>
+  </si>
+  <si>
+    <t>BRD-section</t>
+  </si>
+  <si>
+    <t>FRD-section</t>
+  </si>
+  <si>
+    <t>TS_Loan_001</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TS_Loan_002</t>
+  </si>
+  <si>
+    <t>TS_Loan_003</t>
+  </si>
+  <si>
+    <t>TS_Loan_004</t>
+  </si>
+  <si>
+    <t>TS_Loan_005</t>
+  </si>
+  <si>
+    <t>TS_Loan_006</t>
+  </si>
+  <si>
+    <t>TS_Loan_007</t>
+  </si>
+  <si>
+    <t>TS_Loan_008</t>
+  </si>
+  <si>
+    <t>TS_Loan_009</t>
+  </si>
+  <si>
+    <t>TS_Loan_010</t>
+  </si>
+  <si>
+    <t>TS_Loan_011</t>
+  </si>
+  <si>
+    <t>TS_Loan_012</t>
+  </si>
+  <si>
+    <t>TS_Loan_013</t>
+  </si>
+  <si>
+    <t>TS_Loan_014</t>
+  </si>
+  <si>
+    <t>TS_Loan_015</t>
+  </si>
+  <si>
+    <t>TS_Loan_016</t>
+  </si>
+  <si>
+    <t>TS_Loan_017</t>
+  </si>
+  <si>
+    <t>TS_Loan_018</t>
+  </si>
+  <si>
+    <t>TS_Loan_019</t>
+  </si>
+  <si>
+    <t>TS_Loan_020</t>
+  </si>
+  <si>
+    <t>TS_Loan_021</t>
+  </si>
+  <si>
+    <t>TS_Loan_022</t>
+  </si>
+  <si>
+    <t>TS_Loan_023</t>
+  </si>
+  <si>
+    <t>TS_Loan_024</t>
+  </si>
+  <si>
+    <t>TS_Loan_025</t>
+  </si>
+  <si>
+    <t>TS_Loan_026</t>
+  </si>
+  <si>
+    <t>TS_Loan_027</t>
+  </si>
+  <si>
+    <t>TS_Loan_028</t>
+  </si>
+  <si>
+    <t>TS_Loan_029</t>
+  </si>
+  <si>
+    <t>TS_Loan_030</t>
+  </si>
+  <si>
+    <t>TS_Loan_031</t>
+  </si>
+  <si>
+    <t>TS_Loan_032</t>
+  </si>
+  <si>
+    <t>TS_Loan_033</t>
+  </si>
+  <si>
+    <t>TS_Loan_034</t>
+  </si>
+  <si>
+    <t>TS_Loan_035</t>
+  </si>
+  <si>
+    <t>TS_Loan_036</t>
+  </si>
+  <si>
+    <t>Test Scenarios ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements Traceability Matrix </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,19 +578,53 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -413,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -425,44 +679,99 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -745,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,61 +1327,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>71</v>
       </c>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,237 +1422,502 @@
     <col min="2" max="2" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="24"/>
+    </row>
+    <row r="6" spans="1:2" ht="126" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="24"/>
+    </row>
+    <row r="8" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="26"/>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="26"/>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="26"/>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:2" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="A1" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="e">
+        <f>'Test scenarios'!A2_</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="13"/>
+    </row>
+    <row r="4" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="16" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="L4" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15">
-        <v>4</v>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1320,4 +1926,355 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="str">
+        <f>BRD!A4</f>
+        <v>1. Малогаборитность</v>
+      </c>
+      <c r="C4" s="35" t="str">
+        <f>FRD!A5</f>
+        <v xml:space="preserve">1.1 Размерность </v>
+      </c>
+      <c r="D4" s="34" t="str">
+        <f>'Test scenarios'!A2&amp;'Test scenarios'!B2</f>
+        <v>TS_Loan_001Проверить спецификацию и чертежи устройства</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="34" t="str">
+        <f>'Test scenarios'!A3&amp;'Test scenarios'!B3</f>
+        <v>TS_Loan_002Проверить сборку и разборку</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="34" t="str">
+        <f>'Test scenarios'!A4&amp;'Test scenarios'!B4</f>
+        <v>TS_Loan_003Проверить целостность каждой детали</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="34" t="str">
+        <f>'Test scenarios'!A5&amp;'Test scenarios'!B5</f>
+        <v>TS_Loan_004Сделать визуальный осмотр</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="34" t="str">
+        <f>'Test scenarios'!A6&amp;'Test scenarios'!B6</f>
+        <v>TS_Loan_005Проверить устойчивость кулера на ровной и сухой поверхности</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="34" t="str">
+        <f>'Test scenarios'!A7&amp;'Test scenarios'!B7</f>
+        <v>TS_Loan_006Проверить прочность материала корпуса устройства</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="34" t="str">
+        <f>'Test scenarios'!A8&amp;'Test scenarios'!B8</f>
+        <v xml:space="preserve">TS_Loan_007Проверить шнур питания. </v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="34" t="str">
+        <f>'Test scenarios'!A9&amp;'Test scenarios'!B9</f>
+        <v>TS_Loan_008Проверить вилку от шнура питания.</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="34" t="str">
+        <f>'Test scenarios'!A10&amp;'Test scenarios'!B10</f>
+        <v>TS_Loan_009Проверить подходит ли 10 литровая бутылка с водой.</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
+      <c r="C13" s="37" t="str">
+        <f>FRD!A7</f>
+        <v>1.2 Комплектность</v>
+      </c>
+      <c r="D13" s="34" t="str">
+        <f>'Test scenarios'!A11&amp;'Test scenarios'!B11</f>
+        <v>TS_Loan_010Проверить наличие кранов в кулере</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="34" t="str">
+        <f>'Test scenarios'!A12&amp;'Test scenarios'!B12</f>
+        <v xml:space="preserve">TS_Loan_011Проверить расположение кранов </v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="34" t="str">
+        <f>'Test scenarios'!A13&amp;'Test scenarios'!B13</f>
+        <v>TS_Loan_012Проверить расположение капельный лоток</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="34" t="str">
+        <f>'Test scenarios'!A14&amp;'Test scenarios'!B14</f>
+        <v>TS_Loan_013Проверить растояние между краном и капельным лотком</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="34" t="str">
+        <f>'Test scenarios'!A15&amp;'Test scenarios'!B15</f>
+        <v>TS_Loan_014Проверить вмещаемость капельного лотка на количество стаканов</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="34" t="str">
+        <f>'Test scenarios'!A16&amp;'Test scenarios'!B16</f>
+        <v xml:space="preserve">TS_Loan_015Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="34" t="str">
+        <f>'Test scenarios'!A17&amp;'Test scenarios'!B17</f>
+        <v>TS_Loan_016Проверит отсек для хранение на вмещаемость</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="34" t="str">
+        <f>'Test scenarios'!A18&amp;'Test scenarios'!B18</f>
+        <v>TS_Loan_017Проверить время затраченого на озонирование посуды</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="34" t="str">
+        <f>'Test scenarios'!A19&amp;'Test scenarios'!B19</f>
+        <v>TS_Loan_018Проверить наличее холодильной камеры</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="34" t="str">
+        <f>'Test scenarios'!A20&amp;'Test scenarios'!B20</f>
+        <v>TS_Loan_019Проверить плотно ли закрываеться дверь от холодильной камеры</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="34" t="str">
+        <f>'Test scenarios'!A21&amp;'Test scenarios'!B21</f>
+        <v>TS_Loan_020Проверить вмещаемость холодильной камеры</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="36" t="str">
+        <f>BRD!A6</f>
+        <v>2. Функциональность</v>
+      </c>
+      <c r="C24" s="36" t="str">
+        <f>FRD!A11</f>
+        <v xml:space="preserve">2.1 Функция охлождение </v>
+      </c>
+      <c r="D24" s="34" t="str">
+        <f>'Test scenarios'!A22&amp;'Test scenarios'!B22</f>
+        <v>TS_Loan_021Проверить функциональность выдачи воды из крана</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="34" t="str">
+        <f>'Test scenarios'!A23&amp;'Test scenarios'!B23</f>
+        <v>TS_Loan_022Проверить температуру воды до охлождения и после</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="34" t="str">
+        <f>'Test scenarios'!A24&amp;'Test scenarios'!B24</f>
+        <v>TS_Loan_023Проверить время затраченое на охлождение воды до температуры указаной заказчиком</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="34" t="str">
+        <f>'Test scenarios'!A25&amp;'Test scenarios'!B25</f>
+        <v xml:space="preserve">TS_Loan_024Провирить температуру холодильной камеры до включение и после </v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36" t="str">
+        <f>FRD!A14</f>
+        <v>2.2 Функция подогрева</v>
+      </c>
+      <c r="D28" s="34" t="str">
+        <f>'Test scenarios'!A26&amp;'Test scenarios'!B26</f>
+        <v>TS_Loan_025Проверить функциональность подачи подогретой воды</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="34" t="str">
+        <f>'Test scenarios'!A27&amp;'Test scenarios'!B27</f>
+        <v>TS_Loan_026Проверить температуру воды до подогрева и после</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="34" t="str">
+        <f>'Test scenarios'!A28&amp;'Test scenarios'!B28</f>
+        <v>TS_Loan_027Проверить время затраченое на подогрев воды до температуры указаной заказчиком</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36" t="str">
+        <f>FRD!A16</f>
+        <v>2.3 Функция фильтрации воды</v>
+      </c>
+      <c r="D31" s="34" t="str">
+        <f>'Test scenarios'!A29&amp;'Test scenarios'!B29</f>
+        <v>TS_Loan_028Проверить функциональность фильтрации воды из крана</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="34" t="str">
+        <f>'Test scenarios'!A30&amp;'Test scenarios'!B30</f>
+        <v>TS_Loan_029Проверить воду на очистку до фильтрации и после.</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="36"/>
+      <c r="C33" s="36" t="str">
+        <f>FRD!A18</f>
+        <v>2.4 Функция газации фоды</v>
+      </c>
+      <c r="D33" s="34" t="str">
+        <f>'Test scenarios'!A31&amp;'Test scenarios'!B31</f>
+        <v>TS_Loan_030Проверить функциональность подачи газа в воду</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="34" t="str">
+        <f>'Test scenarios'!A32&amp;'Test scenarios'!B32</f>
+        <v>TS_Loan_031Проверить выдачу воды из крана</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="34" t="str">
+        <f>'Test scenarios'!A33&amp;'Test scenarios'!B33</f>
+        <v>TS_Loan_032Проверить воду до газирования и после</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="36" t="str">
+        <f>BRD!A10</f>
+        <v>3 Доступность</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="34" t="str">
+        <f>'Test scenarios'!A34&amp;'Test scenarios'!B34</f>
+        <v>TS_Loan_033Проверить наличие панели управления</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="34" t="str">
+        <f>'Test scenarios'!A35&amp;'Test scenarios'!B35</f>
+        <v>TS_Loan_034Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="34" t="str">
+        <f>'Test scenarios'!A36&amp;'Test scenarios'!B36</f>
+        <v>TS_Loan_035Проверить соответсвие кнопок функционированию</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="34" t="str">
+        <f>'Test scenarios'!A37&amp;'Test scenarios'!B37</f>
+        <v>TS_Loan_036Проверить расположение панели управления</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Story 9:Changed Testing mobile phone and meat grinder
</commit_message>
<xml_diff>
--- a/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
+++ b/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="209">
   <si>
     <t>Правильность</t>
   </si>
@@ -409,121 +409,247 @@
     <t>FRD-section</t>
   </si>
   <si>
-    <t>TS_Loan_001</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>TS_Loan_002</t>
-  </si>
-  <si>
-    <t>TS_Loan_003</t>
-  </si>
-  <si>
-    <t>TS_Loan_004</t>
-  </si>
-  <si>
-    <t>TS_Loan_005</t>
-  </si>
-  <si>
-    <t>TS_Loan_006</t>
-  </si>
-  <si>
-    <t>TS_Loan_007</t>
-  </si>
-  <si>
-    <t>TS_Loan_008</t>
-  </si>
-  <si>
-    <t>TS_Loan_009</t>
-  </si>
-  <si>
-    <t>TS_Loan_010</t>
-  </si>
-  <si>
-    <t>TS_Loan_011</t>
-  </si>
-  <si>
-    <t>TS_Loan_012</t>
-  </si>
-  <si>
-    <t>TS_Loan_013</t>
-  </si>
-  <si>
-    <t>TS_Loan_014</t>
-  </si>
-  <si>
-    <t>TS_Loan_015</t>
-  </si>
-  <si>
-    <t>TS_Loan_016</t>
-  </si>
-  <si>
-    <t>TS_Loan_017</t>
-  </si>
-  <si>
-    <t>TS_Loan_018</t>
-  </si>
-  <si>
-    <t>TS_Loan_019</t>
-  </si>
-  <si>
-    <t>TS_Loan_020</t>
-  </si>
-  <si>
-    <t>TS_Loan_021</t>
-  </si>
-  <si>
-    <t>TS_Loan_022</t>
-  </si>
-  <si>
-    <t>TS_Loan_023</t>
-  </si>
-  <si>
-    <t>TS_Loan_024</t>
-  </si>
-  <si>
-    <t>TS_Loan_025</t>
-  </si>
-  <si>
-    <t>TS_Loan_026</t>
-  </si>
-  <si>
-    <t>TS_Loan_027</t>
-  </si>
-  <si>
-    <t>TS_Loan_028</t>
-  </si>
-  <si>
-    <t>TS_Loan_029</t>
-  </si>
-  <si>
-    <t>TS_Loan_030</t>
-  </si>
-  <si>
-    <t>TS_Loan_031</t>
-  </si>
-  <si>
-    <t>TS_Loan_032</t>
-  </si>
-  <si>
-    <t>TS_Loan_033</t>
-  </si>
-  <si>
-    <t>TS_Loan_034</t>
-  </si>
-  <si>
-    <t>TS_Loan_035</t>
-  </si>
-  <si>
-    <t>TS_Loan_036</t>
-  </si>
-  <si>
     <t>Test Scenarios ID</t>
   </si>
   <si>
     <t xml:space="preserve">Requirements Traceability Matrix </t>
+  </si>
+  <si>
+    <t>Проверить клапан на входе, если он будет забит песком,будет ли поступать вода в кулер</t>
+  </si>
+  <si>
+    <t>Проверить прочность кранов, если к ним придать силу</t>
+  </si>
+  <si>
+    <t>Будет ли работать кулер если крышка холодильной камеры будет приодкрытой</t>
+  </si>
+  <si>
+    <t>Проверить устойчевость кулера, если убрать одну ножку опоры</t>
+  </si>
+  <si>
+    <t>Будет ли работать кулер если вилку от шнура питания не подключить к сети</t>
+  </si>
+  <si>
+    <t>Будет ли работать кулер если шнур питания повредить</t>
+  </si>
+  <si>
+    <t>Проверить просность капельного лотка, если положить гирю 20 кг</t>
+  </si>
+  <si>
+    <t>Проверить будет ли работать, если компресор будет отключен</t>
+  </si>
+  <si>
+    <t>Проверить если кулер будет лежать горизонтально, будет ли он работать</t>
+  </si>
+  <si>
+    <t>Проверить будет ли работать если кран холодной воды выкрутить</t>
+  </si>
+  <si>
+    <t>Проверить будт ли работа если кран горячей воды будет перекручен на 180 градусов</t>
+  </si>
+  <si>
+    <t>Проверить будет ли работать  озонатор в кулере для воды, если крышку от отсека для посуды убрать</t>
+  </si>
+  <si>
+    <t>Проверить будет ли охлождать воду с температурой 50 градусов за Цельсием</t>
+  </si>
+  <si>
+    <t>Проверить температуру охлождения в холодильной камере, если дверь от камеры будет открыто постоянно</t>
+  </si>
+  <si>
+    <t>Проверить будет ли подача подогретой воды из крана, если кран будет поврежденным</t>
+  </si>
+  <si>
+    <t>Проверить будет ли подогрев воды если ТЕН будет выключен</t>
+  </si>
+  <si>
+    <t>Проверить будет ли выполняться фильтрация, если фильтр будет засорен</t>
+  </si>
+  <si>
+    <t>Проверить будет ли выполняться газирование воды, если балон без газа</t>
+  </si>
+  <si>
+    <t>Проверить будет ли газирование воды, если трубка подачи газа будет повреждена</t>
+  </si>
+  <si>
+    <t>Проверить будет ли выполняться функция, если зажать сразу кнопки разных функций</t>
+  </si>
+  <si>
+    <t>Проверить будет ли выполнять функции кулер, если панель управление будет повреждена</t>
+  </si>
+  <si>
+    <t>TS_Размерность_001</t>
+  </si>
+  <si>
+    <t>TS_Размерность_002</t>
+  </si>
+  <si>
+    <t>TS_Размерность_003</t>
+  </si>
+  <si>
+    <t>TS_Размерность_004</t>
+  </si>
+  <si>
+    <t>TS_Размерность_005</t>
+  </si>
+  <si>
+    <t>TS_Размерность_006</t>
+  </si>
+  <si>
+    <t>TS_Размерность_007</t>
+  </si>
+  <si>
+    <t>TS_Размерность_008</t>
+  </si>
+  <si>
+    <t>TS_Размерность_009</t>
+  </si>
+  <si>
+    <t>TS_Размерность_010</t>
+  </si>
+  <si>
+    <t>TS_Размерность_011</t>
+  </si>
+  <si>
+    <t>TS_Размерность_012</t>
+  </si>
+  <si>
+    <t>TS_Размерность_013</t>
+  </si>
+  <si>
+    <t>TS_Размерность_014</t>
+  </si>
+  <si>
+    <t>TS_Размерность_015</t>
+  </si>
+  <si>
+    <t>TS_Размерность_016</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_017</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_018</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_019</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_020</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_021</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_022</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_023</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_024</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_025</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_026</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_027</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_028</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_029</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_030</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_031</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_032</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_033</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_034</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_035</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_036</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_037</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_038</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_039</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_040</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_041</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_042</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_043</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_044</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_045</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_046</t>
+  </si>
+  <si>
+    <t>TS_Газирование_047</t>
+  </si>
+  <si>
+    <t>TS_Газирование_048</t>
+  </si>
+  <si>
+    <t>TS_Газирование_049</t>
+  </si>
+  <si>
+    <t>TS_Газирование_050</t>
+  </si>
+  <si>
+    <t>TS_Газирование_051</t>
+  </si>
+  <si>
+    <t>TS_Доступность_052</t>
+  </si>
+  <si>
+    <t>TS_Доступность_053</t>
+  </si>
+  <si>
+    <t>TS_Доступность_054</t>
+  </si>
+  <si>
+    <t>TS_Доступность_055</t>
+  </si>
+  <si>
+    <t>TS_Доступность_056</t>
+  </si>
+  <si>
+    <t>TS_Доступность_057</t>
   </si>
 </sst>
 </file>
@@ -693,9 +819,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -714,34 +837,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -771,6 +870,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,10 +1466,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -1354,45 +1480,45 @@
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="29"/>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="31"/>
     </row>
     <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1412,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
@@ -1423,30 +1549,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="29"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="34"/>
     </row>
     <row r="6" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
@@ -1455,10 +1581,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="34"/>
     </row>
     <row r="8" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -1473,83 +1599,83 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="30"/>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="34"/>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="33"/>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="18" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="31"/>
     </row>
     <row r="21" spans="1:2" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="17" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1557,23 +1683,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>129</v>
+      <c r="A1" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>89</v>
@@ -1587,337 +1713,502 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="e">
-        <f>'Test scenarios'!A2_</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="13"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
-    </row>
-    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="13"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+    </row>
+    <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    </row>
+    <row r="15" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    </row>
+    <row r="16" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+    </row>
+    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>151</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1940,338 +2231,338 @@
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="79.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="32" t="s">
-        <v>166</v>
+      <c r="D1" s="23" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>165</v>
+      <c r="D3" s="24" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="str">
+      <c r="B4" s="25" t="str">
         <f>BRD!A4</f>
         <v>1. Малогаборитность</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="26" t="str">
         <f>FRD!A5</f>
         <v xml:space="preserve">1.1 Размерность </v>
       </c>
-      <c r="D4" s="34" t="str">
+      <c r="D4" s="25" t="str">
         <f>'Test scenarios'!A2&amp;'Test scenarios'!B2</f>
-        <v>TS_Loan_001Проверить спецификацию и чертежи устройства</v>
+        <v>TS_Размерность_001Проверить спецификацию и чертежи устройства</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="34" t="str">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25" t="str">
         <f>'Test scenarios'!A3&amp;'Test scenarios'!B3</f>
-        <v>TS_Loan_002Проверить сборку и разборку</v>
+        <v>TS_Размерность_002Проверить сборку и разборку</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="34" t="str">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="25" t="str">
         <f>'Test scenarios'!A4&amp;'Test scenarios'!B4</f>
-        <v>TS_Loan_003Проверить целостность каждой детали</v>
+        <v>TS_Размерность_003Проверить целостность каждой детали</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="34" t="str">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="25" t="str">
         <f>'Test scenarios'!A5&amp;'Test scenarios'!B5</f>
-        <v>TS_Loan_004Сделать визуальный осмотр</v>
+        <v>TS_Размерность_004Сделать визуальный осмотр</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="34" t="str">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="25" t="str">
         <f>'Test scenarios'!A6&amp;'Test scenarios'!B6</f>
-        <v>TS_Loan_005Проверить устойчивость кулера на ровной и сухой поверхности</v>
+        <v>TS_Размерность_005Проверить устойчивость кулера на ровной и сухой поверхности</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="34" t="str">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="25" t="str">
         <f>'Test scenarios'!A7&amp;'Test scenarios'!B7</f>
-        <v>TS_Loan_006Проверить прочность материала корпуса устройства</v>
+        <v>TS_Размерность_006Проверить прочность материала корпуса устройства</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="34" t="str">
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="25" t="str">
         <f>'Test scenarios'!A8&amp;'Test scenarios'!B8</f>
-        <v xml:space="preserve">TS_Loan_007Проверить шнур питания. </v>
+        <v xml:space="preserve">TS_Размерность_007Проверить шнур питания. </v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="34" t="str">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="25" t="str">
         <f>'Test scenarios'!A9&amp;'Test scenarios'!B9</f>
-        <v>TS_Loan_008Проверить вилку от шнура питания.</v>
+        <v>TS_Размерность_008Проверить вилку от шнура питания.</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="34" t="str">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="25" t="str">
         <f>'Test scenarios'!A10&amp;'Test scenarios'!B10</f>
-        <v>TS_Loan_009Проверить подходит ли 10 литровая бутылка с водой.</v>
+        <v>TS_Размерность_009Проверить подходит ли 10 литровая бутылка с водой.</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="37" t="str">
+      <c r="B13" s="27"/>
+      <c r="C13" s="28" t="str">
         <f>FRD!A7</f>
         <v>1.2 Комплектность</v>
       </c>
-      <c r="D13" s="34" t="str">
-        <f>'Test scenarios'!A11&amp;'Test scenarios'!B11</f>
-        <v>TS_Loan_010Проверить наличие кранов в кулере</v>
+      <c r="D13" s="25" t="str">
+        <f>'Test scenarios'!A18&amp;'Test scenarios'!B18</f>
+        <v>TS_Комплектность_017Проверить наличие кранов в кулере</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="34" t="str">
-        <f>'Test scenarios'!A12&amp;'Test scenarios'!B12</f>
-        <v xml:space="preserve">TS_Loan_011Проверить расположение кранов </v>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="25" t="str">
+        <f>'Test scenarios'!A19&amp;'Test scenarios'!B19</f>
+        <v xml:space="preserve">TS_Комплектность_018Проверить расположение кранов </v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="34" t="str">
-        <f>'Test scenarios'!A13&amp;'Test scenarios'!B13</f>
-        <v>TS_Loan_012Проверить расположение капельный лоток</v>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="25" t="str">
+        <f>'Test scenarios'!A20&amp;'Test scenarios'!B20</f>
+        <v>TS_Комплектность_019Проверить расположение капельный лоток</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="34" t="str">
-        <f>'Test scenarios'!A14&amp;'Test scenarios'!B14</f>
-        <v>TS_Loan_013Проверить растояние между краном и капельным лотком</v>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="25" t="str">
+        <f>'Test scenarios'!A21&amp;'Test scenarios'!B21</f>
+        <v>TS_Комплектность_020Проверить растояние между краном и капельным лотком</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="34" t="str">
-        <f>'Test scenarios'!A15&amp;'Test scenarios'!B15</f>
-        <v>TS_Loan_014Проверить вмещаемость капельного лотка на количество стаканов</v>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="25" t="str">
+        <f>'Test scenarios'!A22&amp;'Test scenarios'!B22</f>
+        <v>TS_Комплектность_021Проверить вмещаемость капельного лотка на количество стаканов</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="34" t="str">
-        <f>'Test scenarios'!A16&amp;'Test scenarios'!B16</f>
-        <v xml:space="preserve">TS_Loan_015Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </v>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="25" t="str">
+        <f>'Test scenarios'!A28&amp;'Test scenarios'!B28</f>
+        <v xml:space="preserve">TS_Комплектность_027Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="34" t="str">
-        <f>'Test scenarios'!A17&amp;'Test scenarios'!B17</f>
-        <v>TS_Loan_016Проверит отсек для хранение на вмещаемость</v>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="25" t="str">
+        <f>'Test scenarios'!A29&amp;'Test scenarios'!B29</f>
+        <v>TS_Комплектность_028Проверит отсек для хранение на вмещаемость</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="34" t="str">
-        <f>'Test scenarios'!A18&amp;'Test scenarios'!B18</f>
-        <v>TS_Loan_017Проверить время затраченого на озонирование посуды</v>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="25" t="str">
+        <f>'Test scenarios'!A30&amp;'Test scenarios'!B30</f>
+        <v>TS_Комплектность_029Проверить время затраченого на озонирование посуды</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="34" t="str">
-        <f>'Test scenarios'!A19&amp;'Test scenarios'!B19</f>
-        <v>TS_Loan_018Проверить наличее холодильной камеры</v>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="25" t="str">
+        <f>'Test scenarios'!A31&amp;'Test scenarios'!B31</f>
+        <v>TS_Комплектность_030Проверить наличее холодильной камеры</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="34" t="str">
-        <f>'Test scenarios'!A20&amp;'Test scenarios'!B20</f>
-        <v>TS_Loan_019Проверить плотно ли закрываеться дверь от холодильной камеры</v>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="25" t="str">
+        <f>'Test scenarios'!A32&amp;'Test scenarios'!B32</f>
+        <v>TS_Комплектность_031Проверить плотно ли закрываеться дверь от холодильной камеры</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="34" t="str">
-        <f>'Test scenarios'!A21&amp;'Test scenarios'!B21</f>
-        <v>TS_Loan_020Проверить вмещаемость холодильной камеры</v>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="25" t="str">
+        <f>'Test scenarios'!A33&amp;'Test scenarios'!B33</f>
+        <v>TS_Комплектность_032Проверить вмещаемость холодильной камеры</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="str">
+      <c r="B24" s="27" t="str">
         <f>BRD!A6</f>
         <v>2. Функциональность</v>
       </c>
-      <c r="C24" s="36" t="str">
+      <c r="C24" s="27" t="str">
         <f>FRD!A11</f>
         <v xml:space="preserve">2.1 Функция охлождение </v>
       </c>
-      <c r="D24" s="34" t="str">
-        <f>'Test scenarios'!A22&amp;'Test scenarios'!B22</f>
-        <v>TS_Loan_021Проверить функциональность выдачи воды из крана</v>
+      <c r="D24" s="25" t="str">
+        <f>'Test scenarios'!A34&amp;'Test scenarios'!B34</f>
+        <v>TS_Охлождение_033Проверить функциональность выдачи воды из крана</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="34" t="str">
-        <f>'Test scenarios'!A23&amp;'Test scenarios'!B23</f>
-        <v>TS_Loan_022Проверить температуру воды до охлождения и после</v>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="25" t="str">
+        <f>'Test scenarios'!A35&amp;'Test scenarios'!B35</f>
+        <v>TS_Охлождение_034Проверить температуру воды до охлождения и после</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="34" t="str">
-        <f>'Test scenarios'!A24&amp;'Test scenarios'!B24</f>
-        <v>TS_Loan_023Проверить время затраченое на охлождение воды до температуры указаной заказчиком</v>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="25" t="str">
+        <f>'Test scenarios'!A36&amp;'Test scenarios'!B36</f>
+        <v>TS_Охлождение_035Проверить время затраченое на охлождение воды до температуры указаной заказчиком</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="34" t="str">
-        <f>'Test scenarios'!A25&amp;'Test scenarios'!B25</f>
-        <v xml:space="preserve">TS_Loan_024Провирить температуру холодильной камеры до включение и после </v>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="25" t="str">
+        <f>'Test scenarios'!A38&amp;'Test scenarios'!B38</f>
+        <v xml:space="preserve">TS_Охлождение_037Провирить температуру холодильной камеры до включение и после </v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36" t="str">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27" t="str">
         <f>FRD!A14</f>
         <v>2.2 Функция подогрева</v>
       </c>
-      <c r="D28" s="34" t="str">
-        <f>'Test scenarios'!A26&amp;'Test scenarios'!B26</f>
-        <v>TS_Loan_025Проверить функциональность подачи подогретой воды</v>
+      <c r="D28" s="25" t="str">
+        <f>'Test scenarios'!A40&amp;'Test scenarios'!B40</f>
+        <v>TS_Подогрев_039Проверить функциональность подачи подогретой воды</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="34" t="str">
-        <f>'Test scenarios'!A27&amp;'Test scenarios'!B27</f>
-        <v>TS_Loan_026Проверить температуру воды до подогрева и после</v>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="25" t="str">
+        <f>'Test scenarios'!A41&amp;'Test scenarios'!B41</f>
+        <v>TS_Подогрев_040Проверить температуру воды до подогрева и после</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="34" t="str">
-        <f>'Test scenarios'!A28&amp;'Test scenarios'!B28</f>
-        <v>TS_Loan_027Проверить время затраченое на подогрев воды до температуры указаной заказчиком</v>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="25" t="str">
+        <f>'Test scenarios'!A42&amp;'Test scenarios'!B42</f>
+        <v>TS_Подогрев_041Проверить время затраченое на подогрев воды до температуры указаной заказчиком</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
-      <c r="C31" s="36" t="str">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27" t="str">
         <f>FRD!A16</f>
         <v>2.3 Функция фильтрации воды</v>
       </c>
-      <c r="D31" s="34" t="str">
-        <f>'Test scenarios'!A29&amp;'Test scenarios'!B29</f>
-        <v>TS_Loan_028Проверить функциональность фильтрации воды из крана</v>
+      <c r="D31" s="25" t="str">
+        <f>'Test scenarios'!A45&amp;'Test scenarios'!B45</f>
+        <v>TS_Фильтрация_044Проверить функциональность фильтрации воды из крана</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="34" t="str">
-        <f>'Test scenarios'!A30&amp;'Test scenarios'!B30</f>
-        <v>TS_Loan_029Проверить воду на очистку до фильтрации и после.</v>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="25" t="str">
+        <f>'Test scenarios'!A46&amp;'Test scenarios'!B46</f>
+        <v>TS_Фильтрация_045Проверить воду на очистку до фильтрации и после.</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
-      <c r="C33" s="36" t="str">
+      <c r="B33" s="27"/>
+      <c r="C33" s="27" t="str">
         <f>FRD!A18</f>
         <v>2.4 Функция газации фоды</v>
       </c>
-      <c r="D33" s="34" t="str">
-        <f>'Test scenarios'!A31&amp;'Test scenarios'!B31</f>
-        <v>TS_Loan_030Проверить функциональность подачи газа в воду</v>
+      <c r="D33" s="25" t="str">
+        <f>'Test scenarios'!A48&amp;'Test scenarios'!B48</f>
+        <v>TS_Газирование_047Проверить функциональность подачи газа в воду</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="34" t="str">
-        <f>'Test scenarios'!A32&amp;'Test scenarios'!B32</f>
-        <v>TS_Loan_031Проверить выдачу воды из крана</v>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="25" t="str">
+        <f>'Test scenarios'!A49&amp;'Test scenarios'!B49</f>
+        <v>TS_Газирование_048Проверить выдачу воды из крана</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="34" t="str">
-        <f>'Test scenarios'!A33&amp;'Test scenarios'!B33</f>
-        <v>TS_Loan_032Проверить воду до газирования и после</v>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="25" t="str">
+        <f>'Test scenarios'!A50&amp;'Test scenarios'!B50</f>
+        <v>TS_Газирование_049Проверить воду до газирования и после</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="36" t="str">
+      <c r="B36" s="27" t="str">
         <f>BRD!A10</f>
         <v>3 Доступность</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="34" t="str">
-        <f>'Test scenarios'!A34&amp;'Test scenarios'!B34</f>
-        <v>TS_Loan_033Проверить наличие панели управления</v>
+      <c r="C36" s="27"/>
+      <c r="D36" s="25" t="str">
+        <f>'Test scenarios'!A53&amp;'Test scenarios'!B53</f>
+        <v>TS_Доступность_052Проверить наличие панели управления</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="34" t="str">
-        <f>'Test scenarios'!A35&amp;'Test scenarios'!B35</f>
-        <v>TS_Loan_034Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</v>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="25" t="str">
+        <f>'Test scenarios'!A54&amp;'Test scenarios'!B54</f>
+        <v>TS_Доступность_053Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="34" t="str">
-        <f>'Test scenarios'!A36&amp;'Test scenarios'!B36</f>
-        <v>TS_Loan_035Проверить соответсвие кнопок функционированию</v>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="25" t="str">
+        <f>'Test scenarios'!A55&amp;'Test scenarios'!B55</f>
+        <v>TS_Доступность_054Проверить соответсвие кнопок функционированию</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="34" t="str">
-        <f>'Test scenarios'!A37&amp;'Test scenarios'!B37</f>
-        <v>TS_Loan_036Проверить расположение панели управления</v>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="25" t="str">
+        <f>'Test scenarios'!A56&amp;'Test scenarios'!B56</f>
+        <v>TS_Доступность_055Проверить расположение панели управления</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Story 10:Changed Cooler Traceability Matrix
</commit_message>
<xml_diff>
--- a/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
+++ b/Homework_2/Cooler_requirement_and_Traceability_Matrix_Vlad_Dmytrenko.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="253">
   <si>
     <t>Правильность</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Проверить прочность кранов, если к ним придать силу</t>
   </si>
   <si>
-    <t>Будет ли работать кулер если крышка холодильной камеры будет приодкрытой</t>
-  </si>
-  <si>
     <t>Проверить устойчевость кулера, если убрать одну ножку опоры</t>
   </si>
   <si>
@@ -529,127 +526,262 @@
     <t>TS_Размерность_016</t>
   </si>
   <si>
-    <t>TS_Комплектность_017</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_018</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_019</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_020</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_021</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_022</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_023</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_024</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_025</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_026</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_027</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_028</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_029</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_030</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_031</t>
-  </si>
-  <si>
-    <t>TS_Комплектность_032</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_033</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_034</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_035</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_036</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_037</t>
-  </si>
-  <si>
-    <t>TS_Охлождение_038</t>
-  </si>
-  <si>
-    <t>TS_Подогрев_039</t>
-  </si>
-  <si>
-    <t>TS_Подогрев_040</t>
-  </si>
-  <si>
-    <t>TS_Подогрев_041</t>
-  </si>
-  <si>
-    <t>TS_Подогрев_042</t>
-  </si>
-  <si>
-    <t>TS_Подогрев_043</t>
-  </si>
-  <si>
-    <t>TS_Фильтрация_044</t>
-  </si>
-  <si>
-    <t>TS_Фильтрация_045</t>
-  </si>
-  <si>
-    <t>TS_Фильтрация_046</t>
-  </si>
-  <si>
-    <t>TS_Газирование_047</t>
-  </si>
-  <si>
-    <t>TS_Газирование_048</t>
-  </si>
-  <si>
-    <t>TS_Газирование_049</t>
-  </si>
-  <si>
-    <t>TS_Газирование_050</t>
-  </si>
-  <si>
-    <t>TS_Газирование_051</t>
-  </si>
-  <si>
-    <t>TS_Доступность_052</t>
-  </si>
-  <si>
-    <t>TS_Доступность_053</t>
-  </si>
-  <si>
-    <t>TS_Доступность_054</t>
-  </si>
-  <si>
-    <t>TS_Доступность_055</t>
-  </si>
-  <si>
-    <t>TS_Доступность_056</t>
-  </si>
-  <si>
-    <t>TS_Доступность_057</t>
+    <t>Проверить все товары на складе</t>
+  </si>
+  <si>
+    <t>Проверить с перечисленными деталями в требовании и инструкции</t>
+  </si>
+  <si>
+    <t>Наличие инструкции на английском языке</t>
+  </si>
+  <si>
+    <t>Проверить наличие цветовой индикации на кранах</t>
+  </si>
+  <si>
+    <t>Проверить цвет "синий" присутствует на кране холодной воды</t>
+  </si>
+  <si>
+    <t>Проверить цвет "красный" присутствует на кране горячей воды</t>
+  </si>
+  <si>
+    <t>Будет ли работать кулер если крышка холодильной камеры будет приоткрытой</t>
+  </si>
+  <si>
+    <t>Проверить наличие шнура питания</t>
+  </si>
+  <si>
+    <t xml:space="preserve">есть ли инструкция подключения к сети </t>
+  </si>
+  <si>
+    <t>есть наличие штекера с вилкой</t>
+  </si>
+  <si>
+    <t>шнур питания и штекер с вилкой это одно целое</t>
+  </si>
+  <si>
+    <t>Проверить какой длины шнур питания</t>
+  </si>
+  <si>
+    <t>Проверить прочность шнура питания</t>
+  </si>
+  <si>
+    <t>Если уронить на шнур питания вещь весом 50 кг, будет ли пригодным для подключение к сети</t>
+  </si>
+  <si>
+    <t>какой формы имеет вилка</t>
+  </si>
+  <si>
+    <t>вилка трехконтактная</t>
+  </si>
+  <si>
+    <t>вилка двухконтактная</t>
+  </si>
+  <si>
+    <t>вилка трехконтактная, а розетка двухконтактная</t>
+  </si>
+  <si>
+    <t>вилка двухконтактная, а розетка трехконтактная</t>
+  </si>
+  <si>
+    <t>подключить кулер к напряжению 220 вольт по инструкции</t>
+  </si>
+  <si>
+    <t>подключить кулер к напряжению менее 220 вольт</t>
+  </si>
+  <si>
+    <t>если напряжение будет изменять по шкале от 200 до 300 вольт</t>
+  </si>
+  <si>
+    <t>Если температура подогретого цикла упадет ниже 90 градусов,будет ли водаподогреваться</t>
+  </si>
+  <si>
+    <t>TS_Размерность_017</t>
+  </si>
+  <si>
+    <t>TS_Размерность_018</t>
+  </si>
+  <si>
+    <t>TS_Размерность_019</t>
+  </si>
+  <si>
+    <t>TS_Размерность_020</t>
+  </si>
+  <si>
+    <t>TS_Размерность_021</t>
+  </si>
+  <si>
+    <t>TS_Размерность_022</t>
+  </si>
+  <si>
+    <t>TS_Размерность_023</t>
+  </si>
+  <si>
+    <t>TS_Размерность_024</t>
+  </si>
+  <si>
+    <t>TS_Размерность_025</t>
+  </si>
+  <si>
+    <t>TS_Размерность_026</t>
+  </si>
+  <si>
+    <t>TS_Размерность_027</t>
+  </si>
+  <si>
+    <t>TS_Размерность_028</t>
+  </si>
+  <si>
+    <t>TS_Размерность_029</t>
+  </si>
+  <si>
+    <t>TS_Размерность_030</t>
+  </si>
+  <si>
+    <t>TS_Размерность_031</t>
+  </si>
+  <si>
+    <t>TS_Размерность_032</t>
+  </si>
+  <si>
+    <t>TS_Размерность_033</t>
+  </si>
+  <si>
+    <t>TS_Размерность_034</t>
+  </si>
+  <si>
+    <t>TS_Размерность_035</t>
+  </si>
+  <si>
+    <t>TS_Размерность_036</t>
+  </si>
+  <si>
+    <t>TS_Размерность_037</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_038</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_039</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_040</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_041</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_042</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_043</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_044</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_045</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_046</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_047</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_048</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_049</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_050</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_051</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_052</t>
+  </si>
+  <si>
+    <t>TS_Комплектность_053</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_054</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_055</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_056</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_057</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_058</t>
+  </si>
+  <si>
+    <t>TS_Охлождение_059</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_060</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_061</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_062</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_063</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_064</t>
+  </si>
+  <si>
+    <t>TS_Подогрев_065</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_066</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_067</t>
+  </si>
+  <si>
+    <t>TS_Фильтрация_068</t>
+  </si>
+  <si>
+    <t>TS_Газирование_069</t>
+  </si>
+  <si>
+    <t>TS_Газирование_070</t>
+  </si>
+  <si>
+    <t>TS_Газирование_071</t>
+  </si>
+  <si>
+    <t>TS_Газирование_072</t>
+  </si>
+  <si>
+    <t>TS_Газирование_073</t>
+  </si>
+  <si>
+    <t>TS_Доступность_074</t>
+  </si>
+  <si>
+    <t>TS_Доступность_075</t>
+  </si>
+  <si>
+    <t>TS_Доступность_076</t>
+  </si>
+  <si>
+    <t>TS_Доступность_077</t>
+  </si>
+  <si>
+    <t>TS_Доступность_078</t>
+  </si>
+  <si>
+    <t>TS_Доступность_079</t>
   </si>
 </sst>
 </file>
@@ -793,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -883,20 +1015,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1549,10 +1685,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -1569,10 +1705,10 @@
       <c r="B4" s="29"/>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="35"/>
     </row>
     <row r="6" spans="1:2" ht="126" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
@@ -1581,10 +1717,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="35"/>
     </row>
     <row r="8" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -1605,10 +1741,10 @@
       <c r="B10" s="30"/>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="34"/>
+      <c r="B11" s="35"/>
     </row>
     <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
@@ -1621,10 +1757,10 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="36"/>
     </row>
     <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
@@ -1632,10 +1768,10 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="36"/>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
@@ -1643,10 +1779,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="36"/>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
@@ -1666,16 +1802,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1683,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,505 +1851,711 @@
       <c r="K1" s="8"/>
       <c r="L1" s="37"/>
     </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="37"/>
+    </row>
+    <row r="3" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B3" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="37"/>
+    </row>
+    <row r="4" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L5" s="37"/>
+    </row>
+    <row r="6" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B7" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="19" t="s">
+    <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="19" t="s">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="19" t="s">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" s="19" t="s">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>164</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="B16" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>167</v>
-      </c>
       <c r="B17" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>104</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>112</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>151</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="L1:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2221,17 +2563,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D39"/>
+  <dimension ref="B1:D324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="79.5703125" customWidth="1"/>
+    <col min="4" max="4" width="115.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2250,7 +2592,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="str">
         <f>BRD!A4</f>
         <v>1. Малогаборитность</v>
@@ -2261,7 +2603,7 @@
       </c>
       <c r="D4" s="25" t="str">
         <f>'Test scenarios'!A2&amp;'Test scenarios'!B2</f>
-        <v>TS_Размерность_001Проверить спецификацию и чертежи устройства</v>
+        <v>TS_Размерность_001Проверить все товары на складе</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2269,15 +2611,15 @@
       <c r="C5" s="27"/>
       <c r="D5" s="25" t="str">
         <f>'Test scenarios'!A3&amp;'Test scenarios'!B3</f>
-        <v>TS_Размерность_002Проверить сборку и разборку</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>TS_Размерность_002Проверить с перечисленными деталями в требовании и инструкции</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="25" t="str">
         <f>'Test scenarios'!A4&amp;'Test scenarios'!B4</f>
-        <v>TS_Размерность_003Проверить целостность каждой детали</v>
+        <v>TS_Размерность_003Наличие инструкции на английском языке</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2285,23 +2627,23 @@
       <c r="C7" s="27"/>
       <c r="D7" s="25" t="str">
         <f>'Test scenarios'!A5&amp;'Test scenarios'!B5</f>
-        <v>TS_Размерность_004Сделать визуальный осмотр</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>TS_Размерность_004Проверить спецификацию и чертежи устройства</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="25" t="str">
         <f>'Test scenarios'!A6&amp;'Test scenarios'!B6</f>
-        <v>TS_Размерность_005Проверить устойчивость кулера на ровной и сухой поверхности</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>TS_Размерность_005Проверить сборку и разборку</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="25" t="str">
         <f>'Test scenarios'!A7&amp;'Test scenarios'!B7</f>
-        <v>TS_Размерность_006Проверить прочность материала корпуса устройства</v>
+        <v>TS_Размерность_006Проверить целостность каждой детали</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2309,7 +2651,7 @@
       <c r="C10" s="27"/>
       <c r="D10" s="25" t="str">
         <f>'Test scenarios'!A8&amp;'Test scenarios'!B8</f>
-        <v xml:space="preserve">TS_Размерность_007Проверить шнур питания. </v>
+        <v>TS_Размерность_007Сделать визуальный осмотр</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2317,252 +2659,2048 @@
       <c r="C11" s="27"/>
       <c r="D11" s="25" t="str">
         <f>'Test scenarios'!A9&amp;'Test scenarios'!B9</f>
-        <v>TS_Размерность_008Проверить вилку от шнура питания.</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>TS_Размерность_008Проверить устойчивость кулера на ровной и сухой поверхности</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="25" t="str">
         <f>'Test scenarios'!A10&amp;'Test scenarios'!B10</f>
-        <v>TS_Размерность_009Проверить подходит ли 10 литровая бутылка с водой.</v>
+        <v>TS_Размерность_009Проверить прочность материала корпуса устройства</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="27"/>
-      <c r="C13" s="28" t="str">
-        <f>FRD!A7</f>
-        <v>1.2 Комплектность</v>
-      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="25" t="str">
-        <f>'Test scenarios'!A18&amp;'Test scenarios'!B18</f>
-        <v>TS_Комплектность_017Проверить наличие кранов в кулере</v>
+        <f>'Test scenarios'!A11&amp;'Test scenarios'!B11</f>
+        <v xml:space="preserve">TS_Размерность_010Проверить шнур питания. </v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="25" t="str">
-        <f>'Test scenarios'!A19&amp;'Test scenarios'!B19</f>
-        <v xml:space="preserve">TS_Комплектность_018Проверить расположение кранов </v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A12&amp;'Test scenarios'!B12</f>
+        <v>TS_Размерность_011Проверить вилку от шнура питания.</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="25" t="str">
-        <f>'Test scenarios'!A20&amp;'Test scenarios'!B20</f>
-        <v>TS_Комплектность_019Проверить расположение капельный лоток</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A13&amp;'Test scenarios'!B13</f>
+        <v>TS_Размерность_012Проверить подходит ли 10 литровая бутылка с водой.</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="25" t="str">
-        <f>'Test scenarios'!A21&amp;'Test scenarios'!B21</f>
-        <v>TS_Комплектность_020Проверить растояние между краном и капельным лотком</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A14&amp;'Test scenarios'!B14</f>
+        <v>TS_Размерность_013Проверить устойчевость кулера, если убрать одну ножку опоры</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="25" t="str">
-        <f>'Test scenarios'!A22&amp;'Test scenarios'!B22</f>
-        <v>TS_Комплектность_021Проверить вмещаемость капельного лотка на количество стаканов</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A15&amp;'Test scenarios'!B15</f>
+        <v>TS_Размерность_014Проверить клапан на входе, если он будет забит песком,будет ли поступать вода в кулер</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="25" t="str">
-        <f>'Test scenarios'!A28&amp;'Test scenarios'!B28</f>
-        <v xml:space="preserve">TS_Комплектность_027Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A16&amp;'Test scenarios'!B16</f>
+        <v>TS_Размерность_015Проверить прочность кранов, если к ним придать силу</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
       <c r="D19" s="25" t="str">
-        <f>'Test scenarios'!A29&amp;'Test scenarios'!B29</f>
-        <v>TS_Комплектность_028Проверит отсек для хранение на вмещаемость</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A17&amp;'Test scenarios'!B17</f>
+        <v>TS_Размерность_016Проверить наличие цветовой индикации на кранах</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="25" t="str">
-        <f>'Test scenarios'!A30&amp;'Test scenarios'!B30</f>
-        <v>TS_Комплектность_029Проверить время затраченого на озонирование посуды</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A18&amp;'Test scenarios'!B18</f>
+        <v>TS_Размерность_017Проверить цвет "синий" присутствует на кране холодной воды</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="25" t="str">
-        <f>'Test scenarios'!A31&amp;'Test scenarios'!B31</f>
-        <v>TS_Комплектность_030Проверить наличее холодильной камеры</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A19&amp;'Test scenarios'!B19</f>
+        <v>TS_Размерность_018Проверить цвет "красный" присутствует на кране горячей воды</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="25" t="str">
-        <f>'Test scenarios'!A32&amp;'Test scenarios'!B32</f>
-        <v>TS_Комплектность_031Проверить плотно ли закрываеться дверь от холодильной камеры</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A20&amp;'Test scenarios'!B20</f>
+        <v>TS_Размерность_019Будет ли работать кулер если крышка холодильной камеры будет приоткрытой</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
       <c r="D23" s="25" t="str">
-        <f>'Test scenarios'!A33&amp;'Test scenarios'!B33</f>
-        <v>TS_Комплектность_032Проверить вмещаемость холодильной камеры</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="str">
-        <f>BRD!A6</f>
-        <v>2. Функциональность</v>
-      </c>
-      <c r="C24" s="27" t="str">
-        <f>FRD!A11</f>
-        <v xml:space="preserve">2.1 Функция охлождение </v>
-      </c>
+        <f>'Test scenarios'!A21&amp;'Test scenarios'!B21</f>
+        <v>TS_Размерность_020Проверить наличие шнура питания</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="25" t="str">
-        <f>'Test scenarios'!A34&amp;'Test scenarios'!B34</f>
-        <v>TS_Охлождение_033Проверить функциональность выдачи воды из крана</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A22&amp;'Test scenarios'!B22</f>
+        <v xml:space="preserve">TS_Размерность_021есть ли инструкция подключения к сети </v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="25" t="str">
-        <f>'Test scenarios'!A35&amp;'Test scenarios'!B35</f>
-        <v>TS_Охлождение_034Проверить температуру воды до охлождения и после</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A23&amp;'Test scenarios'!B23</f>
+        <v>TS_Размерность_022есть наличие штекера с вилкой</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="25" t="str">
-        <f>'Test scenarios'!A36&amp;'Test scenarios'!B36</f>
-        <v>TS_Охлождение_035Проверить время затраченое на охлождение воды до температуры указаной заказчиком</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A24&amp;'Test scenarios'!B24</f>
+        <v>TS_Размерность_023шнур питания и штекер с вилкой это одно целое</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="25" t="str">
-        <f>'Test scenarios'!A38&amp;'Test scenarios'!B38</f>
-        <v xml:space="preserve">TS_Охлождение_037Провирить температуру холодильной камеры до включение и после </v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A25&amp;'Test scenarios'!B25</f>
+        <v>TS_Размерность_024Проверить какой длины шнур питания</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="27"/>
-      <c r="C28" s="27" t="str">
-        <f>FRD!A14</f>
-        <v>2.2 Функция подогрева</v>
-      </c>
+      <c r="C28" s="27"/>
       <c r="D28" s="25" t="str">
-        <f>'Test scenarios'!A40&amp;'Test scenarios'!B40</f>
-        <v>TS_Подогрев_039Проверить функциональность подачи подогретой воды</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A26&amp;'Test scenarios'!B26</f>
+        <v>TS_Размерность_025Проверить прочность шнура питания</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="25" t="str">
-        <f>'Test scenarios'!A41&amp;'Test scenarios'!B41</f>
-        <v>TS_Подогрев_040Проверить температуру воды до подогрева и после</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A27&amp;'Test scenarios'!B27</f>
+        <v>TS_Размерность_026Если уронить на шнур питания вещь весом 50 кг, будет ли пригодным для подключение к сети</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="27"/>
       <c r="C30" s="27"/>
       <c r="D30" s="25" t="str">
-        <f>'Test scenarios'!A42&amp;'Test scenarios'!B42</f>
-        <v>TS_Подогрев_041Проверить время затраченое на подогрев воды до температуры указаной заказчиком</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A28&amp;'Test scenarios'!B28</f>
+        <v>TS_Размерность_027какой формы имеет вилка</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="27"/>
-      <c r="C31" s="27" t="str">
-        <f>FRD!A16</f>
-        <v>2.3 Функция фильтрации воды</v>
-      </c>
+      <c r="C31" s="27"/>
       <c r="D31" s="25" t="str">
-        <f>'Test scenarios'!A45&amp;'Test scenarios'!B45</f>
-        <v>TS_Фильтрация_044Проверить функциональность фильтрации воды из крана</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A29&amp;'Test scenarios'!B29</f>
+        <v>TS_Размерность_028вилка трехконтактная</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
       <c r="D32" s="25" t="str">
-        <f>'Test scenarios'!A46&amp;'Test scenarios'!B46</f>
-        <v>TS_Фильтрация_045Проверить воду на очистку до фильтрации и после.</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A30&amp;'Test scenarios'!B30</f>
+        <v>TS_Размерность_029вилка двухконтактная</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="27"/>
-      <c r="C33" s="27" t="str">
-        <f>FRD!A18</f>
-        <v>2.4 Функция газации фоды</v>
-      </c>
+      <c r="C33" s="27"/>
       <c r="D33" s="25" t="str">
-        <f>'Test scenarios'!A48&amp;'Test scenarios'!B48</f>
-        <v>TS_Газирование_047Проверить функциональность подачи газа в воду</v>
+        <f>'Test scenarios'!A31&amp;'Test scenarios'!B31</f>
+        <v>TS_Размерность_030вилка трехконтактная, а розетка двухконтактная</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
       <c r="D34" s="25" t="str">
-        <f>'Test scenarios'!A49&amp;'Test scenarios'!B49</f>
-        <v>TS_Газирование_048Проверить выдачу воды из крана</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A32&amp;'Test scenarios'!B32</f>
+        <v>TS_Размерность_031вилка двухконтактная, а розетка трехконтактная</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="25" t="str">
-        <f>'Test scenarios'!A50&amp;'Test scenarios'!B50</f>
-        <v>TS_Газирование_049Проверить воду до газирования и после</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="27" t="str">
-        <f>BRD!A10</f>
-        <v>3 Доступность</v>
-      </c>
+        <f>'Test scenarios'!A33&amp;'Test scenarios'!B33</f>
+        <v>TS_Размерность_032подключить кулер к напряжению 220 вольт по инструкции</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="27"/>
       <c r="C36" s="27"/>
       <c r="D36" s="25" t="str">
-        <f>'Test scenarios'!A53&amp;'Test scenarios'!B53</f>
-        <v>TS_Доступность_052Проверить наличие панели управления</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="47.25" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A34&amp;'Test scenarios'!B34</f>
+        <v>TS_Размерность_033подключить кулер к напряжению менее 220 вольт</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
       <c r="D37" s="25" t="str">
-        <f>'Test scenarios'!A54&amp;'Test scenarios'!B54</f>
-        <v>TS_Доступность_053Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A35&amp;'Test scenarios'!B35</f>
+        <v>TS_Размерность_034если напряжение будет изменять по шкале от 200 до 300 вольт</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
       <c r="D38" s="25" t="str">
-        <f>'Test scenarios'!A55&amp;'Test scenarios'!B55</f>
-        <v>TS_Доступность_054Проверить соответсвие кнопок функционированию</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+        <f>'Test scenarios'!A36&amp;'Test scenarios'!B36</f>
+        <v>TS_Размерность_035Будет ли работать кулер если вилку от шнура питания не подключить к сети</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
       <c r="D39" s="25" t="str">
+        <f>'Test scenarios'!A37&amp;'Test scenarios'!B37</f>
+        <v>TS_Размерность_036Будет ли работать кулер если шнур питания повредить</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="25" t="str">
+        <f>'Test scenarios'!A38&amp;'Test scenarios'!B38</f>
+        <v>TS_Размерность_037Проверить если кулер будет лежать горизонтально, будет ли он работать</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="27"/>
+      <c r="C41" s="28" t="str">
+        <f>FRD!A7</f>
+        <v>1.2 Комплектность</v>
+      </c>
+      <c r="D41" s="25" t="str">
+        <f>'Test scenarios'!A39&amp;'Test scenarios'!B39</f>
+        <v>TS_Комплектность_038Проверить наличие кранов в кулере</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="25" t="str">
+        <f>'Test scenarios'!A40&amp;'Test scenarios'!B40</f>
+        <v xml:space="preserve">TS_Комплектность_039Проверить расположение кранов </v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="25" t="str">
+        <f>'Test scenarios'!A41&amp;'Test scenarios'!B41</f>
+        <v>TS_Комплектность_040Проверить расположение капельный лоток</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="25" t="str">
+        <f>'Test scenarios'!A42&amp;'Test scenarios'!B42</f>
+        <v>TS_Комплектность_041Проверить растояние между краном и капельным лотком</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="25" t="str">
+        <f>'Test scenarios'!A43&amp;'Test scenarios'!B43</f>
+        <v>TS_Комплектность_042Проверить вмещаемость капельного лотка на количество стаканов</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="25" t="str">
+        <f>'Test scenarios'!A44&amp;'Test scenarios'!B44</f>
+        <v>TS_Комплектность_043Проверить просность капельного лотка, если положить гирю 20 кг</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="25" t="str">
+        <f>'Test scenarios'!A45&amp;'Test scenarios'!B45</f>
+        <v>TS_Комплектность_044Проверить будет ли работать, если компресор будет отключен</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="25" t="str">
+        <f>'Test scenarios'!A46&amp;'Test scenarios'!B46</f>
+        <v>TS_Комплектность_045Проверить будет ли работать если кран холодной воды выкрутить</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="25" t="str">
+        <f>'Test scenarios'!A47&amp;'Test scenarios'!B47</f>
+        <v>TS_Комплектность_046Проверить будт ли работа если кран горячей воды будет перекручен на 180 градусов</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="25" t="str">
+        <f>'Test scenarios'!A48&amp;'Test scenarios'!B48</f>
+        <v>TS_Комплектность_047Проверить будет ли работать  озонатор в кулере для воды, если крышку от отсека для посуды убрать</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="25" t="str">
+        <f>'Test scenarios'!A49&amp;'Test scenarios'!B49</f>
+        <v xml:space="preserve">TS_Комплектность_048Проверить отсек для хранение и озонирование посуды на наличей плотно закрывающей дверки </v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="25" t="str">
+        <f>'Test scenarios'!A50&amp;'Test scenarios'!B50</f>
+        <v>TS_Комплектность_049Проверит отсек для хранение на вмещаемость</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="25" t="str">
+        <f>'Test scenarios'!A51&amp;'Test scenarios'!B51</f>
+        <v>TS_Комплектность_050Проверить время затраченого на озонирование посуды</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="25" t="str">
+        <f>'Test scenarios'!A52&amp;'Test scenarios'!B52</f>
+        <v>TS_Комплектность_051Проверить наличее холодильной камеры</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="25" t="str">
+        <f>'Test scenarios'!A53&amp;'Test scenarios'!B53</f>
+        <v>TS_Комплектность_052Проверить плотно ли закрываеться дверь от холодильной камеры</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="25" t="str">
+        <f>'Test scenarios'!A54&amp;'Test scenarios'!B54</f>
+        <v>TS_Комплектность_053Проверить вмещаемость холодильной камеры</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="27" t="str">
+        <f>BRD!A6</f>
+        <v>2. Функциональность</v>
+      </c>
+      <c r="C57" s="27" t="str">
+        <f>FRD!A11</f>
+        <v xml:space="preserve">2.1 Функция охлождение </v>
+      </c>
+      <c r="D57" s="25" t="str">
+        <f>'Test scenarios'!A55&amp;'Test scenarios'!B55</f>
+        <v>TS_Охлождение_054Проверить функциональность выдачи воды из крана</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="27"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="25" t="str">
         <f>'Test scenarios'!A56&amp;'Test scenarios'!B56</f>
-        <v>TS_Доступность_055Проверить расположение панели управления</v>
+        <v>TS_Охлождение_055Проверить температуру воды до охлождения и после</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="25" t="str">
+        <f>'Test scenarios'!A57&amp;'Test scenarios'!B57</f>
+        <v>TS_Охлождение_056Проверить время затраченое на охлождение воды до температуры указаной заказчиком</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="25" t="str">
+        <f>'Test scenarios'!A58&amp;'Test scenarios'!B58</f>
+        <v>TS_Охлождение_057Проверить будет ли охлождать воду с температурой 50 градусов за Цельсием</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="27"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="25" t="str">
+        <f>'Test scenarios'!A59&amp;'Test scenarios'!B59</f>
+        <v xml:space="preserve">TS_Охлождение_058Провирить температуру холодильной камеры до включение и после </v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="25" t="str">
+        <f>'Test scenarios'!A60&amp;'Test scenarios'!B60</f>
+        <v>TS_Охлождение_059Проверить температуру охлождения в холодильной камере, если дверь от камеры будет открыто постоянно</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="27"/>
+      <c r="C63" s="27" t="str">
+        <f>FRD!A14</f>
+        <v>2.2 Функция подогрева</v>
+      </c>
+      <c r="D63" s="25" t="str">
+        <f>'Test scenarios'!A61&amp;'Test scenarios'!B61</f>
+        <v>TS_Подогрев_060Если температура подогретого цикла упадет ниже 90 градусов,будет ли водаподогреваться</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="25" t="str">
+        <f>'Test scenarios'!A62&amp;'Test scenarios'!B62</f>
+        <v>TS_Подогрев_061Проверить функциональность подачи подогретой воды</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="25" t="str">
+        <f>'Test scenarios'!A63&amp;'Test scenarios'!B63</f>
+        <v>TS_Подогрев_062Проверить температуру воды до подогрева и после</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B66" s="38"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="25" t="str">
+        <f>'Test scenarios'!A64&amp;'Test scenarios'!B64</f>
+        <v>TS_Подогрев_063Проверить время затраченое на подогрев воды до температуры указаной заказчиком</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="25" t="str">
+        <f>'Test scenarios'!A65&amp;'Test scenarios'!B65</f>
+        <v>TS_Подогрев_064Проверить будет ли подача подогретой воды из крана, если кран будет поврежденным</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="25" t="str">
+        <f>'Test scenarios'!A66&amp;'Test scenarios'!B66</f>
+        <v>TS_Подогрев_065Проверить будет ли подогрев воды если ТЕН будет выключен</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="27"/>
+      <c r="C69" s="27" t="str">
+        <f>FRD!A16</f>
+        <v>2.3 Функция фильтрации воды</v>
+      </c>
+      <c r="D69" s="25" t="str">
+        <f>'Test scenarios'!A67&amp;'Test scenarios'!B67</f>
+        <v>TS_Фильтрация_066Проверить функциональность фильтрации воды из крана</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="25" t="str">
+        <f>'Test scenarios'!A68&amp;'Test scenarios'!B68</f>
+        <v>TS_Фильтрация_067Проверить воду на очистку до фильтрации и после.</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="25" t="str">
+        <f>'Test scenarios'!A69&amp;'Test scenarios'!B69</f>
+        <v>TS_Фильтрация_068Проверить будет ли выполняться фильтрация, если фильтр будет засорен</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="38"/>
+      <c r="C72" s="27" t="str">
+        <f>FRD!A18</f>
+        <v>2.4 Функция газации фоды</v>
+      </c>
+      <c r="D72" s="25" t="str">
+        <f>'Test scenarios'!A70&amp;'Test scenarios'!B70</f>
+        <v>TS_Газирование_069Проверить функциональность подачи газа в воду</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="25" t="str">
+        <f>'Test scenarios'!A71&amp;'Test scenarios'!B71</f>
+        <v>TS_Газирование_070Проверить выдачу воды из крана</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="25" t="str">
+        <f>'Test scenarios'!A72&amp;'Test scenarios'!B72</f>
+        <v>TS_Газирование_071Проверить воду до газирования и после</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="25" t="str">
+        <f>'Test scenarios'!A73&amp;'Test scenarios'!B73</f>
+        <v>TS_Газирование_072Проверить будет ли выполняться газирование воды, если балон без газа</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="25" t="str">
+        <f>'Test scenarios'!A74&amp;'Test scenarios'!B74</f>
+        <v>TS_Газирование_073Проверить будет ли газирование воды, если трубка подачи газа будет повреждена</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B77" s="27" t="str">
+        <f>BRD!A10</f>
+        <v>3 Доступность</v>
+      </c>
+      <c r="C77" s="38"/>
+      <c r="D77" s="25" t="str">
+        <f>'Test scenarios'!A75&amp;'Test scenarios'!B75</f>
+        <v>TS_Доступность_074Проверить наличие панели управления</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="25" t="str">
+        <f>'Test scenarios'!A76&amp;'Test scenarios'!B76</f>
+        <v>TS_Доступность_075Проверить маркировку функционирования подачи охложденой, подогретой, газированой и фильтрованой воды</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="25" t="str">
+        <f>'Test scenarios'!A77&amp;'Test scenarios'!B77</f>
+        <v>TS_Доступность_076Проверить соответсвие кнопок функционированию</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="25" t="str">
+        <f>'Test scenarios'!A78&amp;'Test scenarios'!B78</f>
+        <v>TS_Доступность_077Проверить расположение панели управления</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="25" t="str">
+        <f>'Test scenarios'!A79&amp;'Test scenarios'!B79</f>
+        <v>TS_Доступность_078Проверить будет ли выполняться функция, если зажать сразу кнопки разных функций</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="25" t="str">
+        <f>'Test scenarios'!A80&amp;'Test scenarios'!B80</f>
+        <v>TS_Доступность_079Проверить будет ли выполнять функции кулер, если панель управление будет повреждена</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D83" s="39" t="str">
+        <f>'Test scenarios'!A81&amp;'Test scenarios'!B81</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D84" s="39" t="str">
+        <f>'Test scenarios'!A82&amp;'Test scenarios'!B82</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D85" s="39" t="str">
+        <f>'Test scenarios'!A83&amp;'Test scenarios'!B83</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D86" s="39" t="str">
+        <f>'Test scenarios'!A84&amp;'Test scenarios'!B84</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D87" s="39" t="str">
+        <f>'Test scenarios'!A85&amp;'Test scenarios'!B85</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D88" s="39" t="str">
+        <f>'Test scenarios'!A86&amp;'Test scenarios'!B86</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D89" s="39" t="str">
+        <f>'Test scenarios'!A87&amp;'Test scenarios'!B87</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D90" s="39" t="str">
+        <f>'Test scenarios'!A88&amp;'Test scenarios'!B88</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D91" s="39" t="str">
+        <f>'Test scenarios'!A89&amp;'Test scenarios'!B89</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D92" s="39" t="str">
+        <f>'Test scenarios'!A90&amp;'Test scenarios'!B90</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D93" s="39" t="str">
+        <f>'Test scenarios'!A91&amp;'Test scenarios'!B91</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D94" s="39" t="str">
+        <f>'Test scenarios'!A92&amp;'Test scenarios'!B92</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D95" s="39" t="str">
+        <f>'Test scenarios'!A93&amp;'Test scenarios'!B93</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D96" s="39" t="str">
+        <f>'Test scenarios'!A94&amp;'Test scenarios'!B94</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D97" s="39" t="str">
+        <f>'Test scenarios'!A95&amp;'Test scenarios'!B95</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D98" s="39" t="str">
+        <f>'Test scenarios'!A96&amp;'Test scenarios'!B96</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D99" s="39" t="str">
+        <f>'Test scenarios'!A97&amp;'Test scenarios'!B97</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D100" s="39" t="str">
+        <f>'Test scenarios'!A98&amp;'Test scenarios'!B98</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D101" s="39" t="str">
+        <f>'Test scenarios'!A99&amp;'Test scenarios'!B99</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D102" s="39" t="str">
+        <f>'Test scenarios'!A100&amp;'Test scenarios'!B100</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D103" s="39" t="str">
+        <f>'Test scenarios'!A101&amp;'Test scenarios'!B101</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D104" s="39" t="str">
+        <f>'Test scenarios'!A102&amp;'Test scenarios'!B102</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D105" s="39" t="str">
+        <f>'Test scenarios'!A103&amp;'Test scenarios'!B103</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D106" s="39" t="str">
+        <f>'Test scenarios'!A104&amp;'Test scenarios'!B104</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D107" s="39" t="str">
+        <f>'Test scenarios'!A105&amp;'Test scenarios'!B105</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D108" s="39" t="str">
+        <f>'Test scenarios'!A106&amp;'Test scenarios'!B106</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D109" s="39" t="str">
+        <f>'Test scenarios'!A107&amp;'Test scenarios'!B107</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D110" s="39" t="str">
+        <f>'Test scenarios'!A108&amp;'Test scenarios'!B108</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D111" s="39" t="str">
+        <f>'Test scenarios'!A109&amp;'Test scenarios'!B109</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D112" s="39" t="str">
+        <f>'Test scenarios'!A110&amp;'Test scenarios'!B110</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D113" s="39" t="str">
+        <f>'Test scenarios'!A111&amp;'Test scenarios'!B111</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D114" s="39" t="str">
+        <f>'Test scenarios'!A112&amp;'Test scenarios'!B112</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D115" s="39" t="str">
+        <f>'Test scenarios'!A113&amp;'Test scenarios'!B113</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D116" s="39" t="str">
+        <f>'Test scenarios'!A114&amp;'Test scenarios'!B114</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D117" s="39" t="str">
+        <f>'Test scenarios'!A115&amp;'Test scenarios'!B115</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D118" s="39" t="str">
+        <f>'Test scenarios'!A116&amp;'Test scenarios'!B116</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D119" s="39" t="str">
+        <f>'Test scenarios'!A117&amp;'Test scenarios'!B117</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D120" s="39" t="str">
+        <f>'Test scenarios'!A118&amp;'Test scenarios'!B118</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D121" s="39" t="str">
+        <f>'Test scenarios'!A119&amp;'Test scenarios'!B119</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D122" s="39" t="str">
+        <f>'Test scenarios'!A120&amp;'Test scenarios'!B120</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D123" s="39" t="str">
+        <f>'Test scenarios'!A121&amp;'Test scenarios'!B121</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D124" s="39" t="str">
+        <f>'Test scenarios'!A122&amp;'Test scenarios'!B122</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D125" s="39" t="str">
+        <f>'Test scenarios'!A123&amp;'Test scenarios'!B123</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D126" s="39" t="str">
+        <f>'Test scenarios'!A124&amp;'Test scenarios'!B124</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D127" s="39" t="str">
+        <f>'Test scenarios'!A125&amp;'Test scenarios'!B125</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D128" s="39" t="str">
+        <f>'Test scenarios'!A126&amp;'Test scenarios'!B126</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D129" s="39" t="str">
+        <f>'Test scenarios'!A127&amp;'Test scenarios'!B127</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D130" s="39" t="str">
+        <f>'Test scenarios'!A128&amp;'Test scenarios'!B128</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D131" s="39" t="str">
+        <f>'Test scenarios'!A129&amp;'Test scenarios'!B129</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D132" s="39" t="str">
+        <f>'Test scenarios'!A130&amp;'Test scenarios'!B130</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D133" s="39" t="str">
+        <f>'Test scenarios'!A131&amp;'Test scenarios'!B131</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D134" s="39" t="str">
+        <f>'Test scenarios'!A132&amp;'Test scenarios'!B132</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D135" s="39" t="str">
+        <f>'Test scenarios'!A133&amp;'Test scenarios'!B133</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D136" s="39" t="str">
+        <f>'Test scenarios'!A134&amp;'Test scenarios'!B134</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D137" s="39" t="str">
+        <f>'Test scenarios'!A135&amp;'Test scenarios'!B135</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D138" s="39" t="str">
+        <f>'Test scenarios'!A136&amp;'Test scenarios'!B136</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D139" s="39" t="str">
+        <f>'Test scenarios'!A137&amp;'Test scenarios'!B137</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D140" s="39" t="str">
+        <f>'Test scenarios'!A138&amp;'Test scenarios'!B138</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D141" s="39" t="str">
+        <f>'Test scenarios'!A139&amp;'Test scenarios'!B139</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D142" s="39" t="str">
+        <f>'Test scenarios'!A140&amp;'Test scenarios'!B140</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D143" s="39" t="str">
+        <f>'Test scenarios'!A141&amp;'Test scenarios'!B141</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D144" s="39" t="str">
+        <f>'Test scenarios'!A142&amp;'Test scenarios'!B142</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D145" s="39" t="str">
+        <f>'Test scenarios'!A143&amp;'Test scenarios'!B143</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D146" s="39" t="str">
+        <f>'Test scenarios'!A144&amp;'Test scenarios'!B144</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D147" s="39" t="str">
+        <f>'Test scenarios'!A145&amp;'Test scenarios'!B145</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D148" s="39" t="str">
+        <f>'Test scenarios'!A146&amp;'Test scenarios'!B146</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D149" s="39" t="str">
+        <f>'Test scenarios'!A147&amp;'Test scenarios'!B147</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D150" s="39" t="str">
+        <f>'Test scenarios'!A148&amp;'Test scenarios'!B148</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D151" s="39" t="str">
+        <f>'Test scenarios'!A149&amp;'Test scenarios'!B149</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D152" s="39" t="str">
+        <f>'Test scenarios'!A150&amp;'Test scenarios'!B150</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D153" s="39" t="str">
+        <f>'Test scenarios'!A151&amp;'Test scenarios'!B151</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D154" s="39" t="str">
+        <f>'Test scenarios'!A152&amp;'Test scenarios'!B152</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D155" s="39" t="str">
+        <f>'Test scenarios'!A153&amp;'Test scenarios'!B153</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D156" s="39" t="str">
+        <f>'Test scenarios'!A154&amp;'Test scenarios'!B154</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D157" s="39" t="str">
+        <f>'Test scenarios'!A155&amp;'Test scenarios'!B155</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D158" s="39" t="str">
+        <f>'Test scenarios'!A156&amp;'Test scenarios'!B156</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D159" s="39" t="str">
+        <f>'Test scenarios'!A157&amp;'Test scenarios'!B157</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D160" s="39" t="str">
+        <f>'Test scenarios'!A158&amp;'Test scenarios'!B158</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D161" s="39" t="str">
+        <f>'Test scenarios'!A159&amp;'Test scenarios'!B159</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D162" s="39" t="str">
+        <f>'Test scenarios'!A160&amp;'Test scenarios'!B160</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D163" s="39" t="str">
+        <f>'Test scenarios'!A161&amp;'Test scenarios'!B161</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D164" s="39" t="str">
+        <f>'Test scenarios'!A162&amp;'Test scenarios'!B162</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D165" s="39" t="str">
+        <f>'Test scenarios'!A163&amp;'Test scenarios'!B163</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D166" s="39" t="str">
+        <f>'Test scenarios'!A164&amp;'Test scenarios'!B164</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D167" s="39" t="str">
+        <f>'Test scenarios'!A165&amp;'Test scenarios'!B165</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D168" s="39" t="str">
+        <f>'Test scenarios'!A166&amp;'Test scenarios'!B166</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D169" s="39" t="str">
+        <f>'Test scenarios'!A167&amp;'Test scenarios'!B167</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D170" s="39" t="str">
+        <f>'Test scenarios'!A168&amp;'Test scenarios'!B168</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D171" s="39" t="str">
+        <f>'Test scenarios'!A169&amp;'Test scenarios'!B169</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D172" s="39" t="str">
+        <f>'Test scenarios'!A170&amp;'Test scenarios'!B170</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D173" s="39" t="str">
+        <f>'Test scenarios'!A171&amp;'Test scenarios'!B171</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D174" s="39" t="str">
+        <f>'Test scenarios'!A172&amp;'Test scenarios'!B172</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D175" s="39" t="str">
+        <f>'Test scenarios'!A173&amp;'Test scenarios'!B173</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D176" s="39" t="str">
+        <f>'Test scenarios'!A174&amp;'Test scenarios'!B174</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D177" s="39" t="str">
+        <f>'Test scenarios'!A175&amp;'Test scenarios'!B175</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D178" s="39" t="str">
+        <f>'Test scenarios'!A176&amp;'Test scenarios'!B176</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D179" s="39" t="str">
+        <f>'Test scenarios'!A177&amp;'Test scenarios'!B177</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D180" s="39" t="str">
+        <f>'Test scenarios'!A178&amp;'Test scenarios'!B178</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D181" s="39" t="str">
+        <f>'Test scenarios'!A179&amp;'Test scenarios'!B179</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D182" s="39" t="str">
+        <f>'Test scenarios'!A180&amp;'Test scenarios'!B180</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D183" s="39" t="str">
+        <f>'Test scenarios'!A181&amp;'Test scenarios'!B181</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D184" s="39" t="str">
+        <f>'Test scenarios'!A182&amp;'Test scenarios'!B182</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D185" s="39" t="str">
+        <f>'Test scenarios'!A183&amp;'Test scenarios'!B183</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D186" s="39" t="str">
+        <f>'Test scenarios'!A184&amp;'Test scenarios'!B184</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D187" s="39" t="str">
+        <f>'Test scenarios'!A185&amp;'Test scenarios'!B185</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D188" s="39" t="str">
+        <f>'Test scenarios'!A186&amp;'Test scenarios'!B186</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D189" s="39" t="str">
+        <f>'Test scenarios'!A187&amp;'Test scenarios'!B187</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D190" s="39" t="str">
+        <f>'Test scenarios'!A188&amp;'Test scenarios'!B188</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D191" s="39" t="str">
+        <f>'Test scenarios'!A189&amp;'Test scenarios'!B189</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D192" s="39" t="str">
+        <f>'Test scenarios'!A190&amp;'Test scenarios'!B190</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D193" s="39" t="str">
+        <f>'Test scenarios'!A191&amp;'Test scenarios'!B191</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D194" s="39" t="str">
+        <f>'Test scenarios'!A192&amp;'Test scenarios'!B192</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D195" s="39" t="str">
+        <f>'Test scenarios'!A193&amp;'Test scenarios'!B193</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D196" s="39" t="str">
+        <f>'Test scenarios'!A194&amp;'Test scenarios'!B194</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D197" s="39" t="str">
+        <f>'Test scenarios'!A195&amp;'Test scenarios'!B195</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D198" s="39" t="str">
+        <f>'Test scenarios'!A196&amp;'Test scenarios'!B196</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D199" s="39" t="str">
+        <f>'Test scenarios'!A197&amp;'Test scenarios'!B197</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D200" s="39" t="str">
+        <f>'Test scenarios'!A198&amp;'Test scenarios'!B198</f>
+        <v/>
+      </c>
+    </row>
+    <row r="201" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D201" s="39" t="str">
+        <f>'Test scenarios'!A199&amp;'Test scenarios'!B199</f>
+        <v/>
+      </c>
+    </row>
+    <row r="202" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D202" s="39" t="str">
+        <f>'Test scenarios'!A200&amp;'Test scenarios'!B200</f>
+        <v/>
+      </c>
+    </row>
+    <row r="203" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D203" s="39" t="str">
+        <f>'Test scenarios'!A201&amp;'Test scenarios'!B201</f>
+        <v/>
+      </c>
+    </row>
+    <row r="204" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D204" s="39" t="str">
+        <f>'Test scenarios'!A202&amp;'Test scenarios'!B202</f>
+        <v/>
+      </c>
+    </row>
+    <row r="205" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D205" s="39" t="str">
+        <f>'Test scenarios'!A203&amp;'Test scenarios'!B203</f>
+        <v/>
+      </c>
+    </row>
+    <row r="206" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D206" s="39" t="str">
+        <f>'Test scenarios'!A204&amp;'Test scenarios'!B204</f>
+        <v/>
+      </c>
+    </row>
+    <row r="207" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D207" s="39" t="str">
+        <f>'Test scenarios'!A205&amp;'Test scenarios'!B205</f>
+        <v/>
+      </c>
+    </row>
+    <row r="208" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D208" s="39" t="str">
+        <f>'Test scenarios'!A206&amp;'Test scenarios'!B206</f>
+        <v/>
+      </c>
+    </row>
+    <row r="209" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D209" s="39" t="str">
+        <f>'Test scenarios'!A207&amp;'Test scenarios'!B207</f>
+        <v/>
+      </c>
+    </row>
+    <row r="210" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D210" s="39" t="str">
+        <f>'Test scenarios'!A208&amp;'Test scenarios'!B208</f>
+        <v/>
+      </c>
+    </row>
+    <row r="211" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D211" s="39" t="str">
+        <f>'Test scenarios'!A209&amp;'Test scenarios'!B209</f>
+        <v/>
+      </c>
+    </row>
+    <row r="212" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D212" s="39" t="str">
+        <f>'Test scenarios'!A210&amp;'Test scenarios'!B210</f>
+        <v/>
+      </c>
+    </row>
+    <row r="213" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D213" s="39" t="str">
+        <f>'Test scenarios'!A211&amp;'Test scenarios'!B211</f>
+        <v/>
+      </c>
+    </row>
+    <row r="214" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D214" s="39" t="str">
+        <f>'Test scenarios'!A212&amp;'Test scenarios'!B212</f>
+        <v/>
+      </c>
+    </row>
+    <row r="215" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D215" s="39" t="str">
+        <f>'Test scenarios'!A213&amp;'Test scenarios'!B213</f>
+        <v/>
+      </c>
+    </row>
+    <row r="216" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D216" s="39" t="str">
+        <f>'Test scenarios'!A214&amp;'Test scenarios'!B214</f>
+        <v/>
+      </c>
+    </row>
+    <row r="217" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D217" s="39" t="str">
+        <f>'Test scenarios'!A215&amp;'Test scenarios'!B215</f>
+        <v/>
+      </c>
+    </row>
+    <row r="218" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D218" s="39" t="str">
+        <f>'Test scenarios'!A216&amp;'Test scenarios'!B216</f>
+        <v/>
+      </c>
+    </row>
+    <row r="219" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D219" s="39" t="str">
+        <f>'Test scenarios'!A217&amp;'Test scenarios'!B217</f>
+        <v/>
+      </c>
+    </row>
+    <row r="220" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D220" s="39" t="str">
+        <f>'Test scenarios'!A218&amp;'Test scenarios'!B218</f>
+        <v/>
+      </c>
+    </row>
+    <row r="221" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D221" s="39" t="str">
+        <f>'Test scenarios'!A219&amp;'Test scenarios'!B219</f>
+        <v/>
+      </c>
+    </row>
+    <row r="222" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D222" s="39" t="str">
+        <f>'Test scenarios'!A220&amp;'Test scenarios'!B220</f>
+        <v/>
+      </c>
+    </row>
+    <row r="223" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D223" s="39" t="str">
+        <f>'Test scenarios'!A221&amp;'Test scenarios'!B221</f>
+        <v/>
+      </c>
+    </row>
+    <row r="224" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D224" s="39" t="str">
+        <f>'Test scenarios'!A222&amp;'Test scenarios'!B222</f>
+        <v/>
+      </c>
+    </row>
+    <row r="225" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D225" s="39" t="str">
+        <f>'Test scenarios'!A223&amp;'Test scenarios'!B223</f>
+        <v/>
+      </c>
+    </row>
+    <row r="226" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D226" s="39" t="str">
+        <f>'Test scenarios'!A224&amp;'Test scenarios'!B224</f>
+        <v/>
+      </c>
+    </row>
+    <row r="227" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D227" s="39" t="str">
+        <f>'Test scenarios'!A225&amp;'Test scenarios'!B225</f>
+        <v/>
+      </c>
+    </row>
+    <row r="228" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D228" s="39" t="str">
+        <f>'Test scenarios'!A226&amp;'Test scenarios'!B226</f>
+        <v/>
+      </c>
+    </row>
+    <row r="229" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D229" s="39" t="str">
+        <f>'Test scenarios'!A227&amp;'Test scenarios'!B227</f>
+        <v/>
+      </c>
+    </row>
+    <row r="230" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D230" s="39" t="str">
+        <f>'Test scenarios'!A228&amp;'Test scenarios'!B228</f>
+        <v/>
+      </c>
+    </row>
+    <row r="231" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D231" s="39" t="str">
+        <f>'Test scenarios'!A229&amp;'Test scenarios'!B229</f>
+        <v/>
+      </c>
+    </row>
+    <row r="232" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D232" s="39" t="str">
+        <f>'Test scenarios'!A230&amp;'Test scenarios'!B230</f>
+        <v/>
+      </c>
+    </row>
+    <row r="233" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D233" s="39" t="str">
+        <f>'Test scenarios'!A231&amp;'Test scenarios'!B231</f>
+        <v/>
+      </c>
+    </row>
+    <row r="234" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D234" s="39" t="str">
+        <f>'Test scenarios'!A232&amp;'Test scenarios'!B232</f>
+        <v/>
+      </c>
+    </row>
+    <row r="235" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D235" s="39" t="str">
+        <f>'Test scenarios'!A233&amp;'Test scenarios'!B233</f>
+        <v/>
+      </c>
+    </row>
+    <row r="236" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D236" s="39" t="str">
+        <f>'Test scenarios'!A234&amp;'Test scenarios'!B234</f>
+        <v/>
+      </c>
+    </row>
+    <row r="237" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D237" s="39" t="str">
+        <f>'Test scenarios'!A235&amp;'Test scenarios'!B235</f>
+        <v/>
+      </c>
+    </row>
+    <row r="238" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D238" s="39" t="str">
+        <f>'Test scenarios'!A236&amp;'Test scenarios'!B236</f>
+        <v/>
+      </c>
+    </row>
+    <row r="239" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D239" s="39" t="str">
+        <f>'Test scenarios'!A237&amp;'Test scenarios'!B237</f>
+        <v/>
+      </c>
+    </row>
+    <row r="240" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D240" s="39" t="str">
+        <f>'Test scenarios'!A238&amp;'Test scenarios'!B238</f>
+        <v/>
+      </c>
+    </row>
+    <row r="241" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D241" s="39" t="str">
+        <f>'Test scenarios'!A239&amp;'Test scenarios'!B239</f>
+        <v/>
+      </c>
+    </row>
+    <row r="242" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D242" s="39" t="str">
+        <f>'Test scenarios'!A240&amp;'Test scenarios'!B240</f>
+        <v/>
+      </c>
+    </row>
+    <row r="243" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D243" s="39" t="str">
+        <f>'Test scenarios'!A241&amp;'Test scenarios'!B241</f>
+        <v/>
+      </c>
+    </row>
+    <row r="244" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D244" s="39" t="str">
+        <f>'Test scenarios'!A242&amp;'Test scenarios'!B242</f>
+        <v/>
+      </c>
+    </row>
+    <row r="245" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D245" s="39" t="str">
+        <f>'Test scenarios'!A243&amp;'Test scenarios'!B243</f>
+        <v/>
+      </c>
+    </row>
+    <row r="246" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D246" s="39" t="str">
+        <f>'Test scenarios'!A244&amp;'Test scenarios'!B244</f>
+        <v/>
+      </c>
+    </row>
+    <row r="247" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D247" s="39" t="str">
+        <f>'Test scenarios'!A245&amp;'Test scenarios'!B245</f>
+        <v/>
+      </c>
+    </row>
+    <row r="248" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D248" s="39" t="str">
+        <f>'Test scenarios'!A246&amp;'Test scenarios'!B246</f>
+        <v/>
+      </c>
+    </row>
+    <row r="249" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D249" s="39" t="str">
+        <f>'Test scenarios'!A247&amp;'Test scenarios'!B247</f>
+        <v/>
+      </c>
+    </row>
+    <row r="250" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D250" s="39" t="str">
+        <f>'Test scenarios'!A248&amp;'Test scenarios'!B248</f>
+        <v/>
+      </c>
+    </row>
+    <row r="251" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D251" s="39" t="str">
+        <f>'Test scenarios'!A249&amp;'Test scenarios'!B249</f>
+        <v/>
+      </c>
+    </row>
+    <row r="252" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D252" s="39" t="str">
+        <f>'Test scenarios'!A250&amp;'Test scenarios'!B250</f>
+        <v/>
+      </c>
+    </row>
+    <row r="253" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D253" s="39" t="str">
+        <f>'Test scenarios'!A251&amp;'Test scenarios'!B251</f>
+        <v/>
+      </c>
+    </row>
+    <row r="254" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D254" s="39" t="str">
+        <f>'Test scenarios'!A252&amp;'Test scenarios'!B252</f>
+        <v/>
+      </c>
+    </row>
+    <row r="255" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D255" s="39" t="str">
+        <f>'Test scenarios'!A253&amp;'Test scenarios'!B253</f>
+        <v/>
+      </c>
+    </row>
+    <row r="256" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D256" s="39" t="str">
+        <f>'Test scenarios'!A254&amp;'Test scenarios'!B254</f>
+        <v/>
+      </c>
+    </row>
+    <row r="257" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D257" s="39" t="str">
+        <f>'Test scenarios'!A255&amp;'Test scenarios'!B255</f>
+        <v/>
+      </c>
+    </row>
+    <row r="258" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D258" s="39" t="str">
+        <f>'Test scenarios'!A256&amp;'Test scenarios'!B256</f>
+        <v/>
+      </c>
+    </row>
+    <row r="259" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D259" s="39" t="str">
+        <f>'Test scenarios'!A257&amp;'Test scenarios'!B257</f>
+        <v/>
+      </c>
+    </row>
+    <row r="260" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D260" s="39" t="str">
+        <f>'Test scenarios'!A258&amp;'Test scenarios'!B258</f>
+        <v/>
+      </c>
+    </row>
+    <row r="261" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D261" s="39" t="str">
+        <f>'Test scenarios'!A259&amp;'Test scenarios'!B259</f>
+        <v/>
+      </c>
+    </row>
+    <row r="262" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D262" s="39" t="str">
+        <f>'Test scenarios'!A260&amp;'Test scenarios'!B260</f>
+        <v/>
+      </c>
+    </row>
+    <row r="263" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D263" s="39" t="str">
+        <f>'Test scenarios'!A261&amp;'Test scenarios'!B261</f>
+        <v/>
+      </c>
+    </row>
+    <row r="264" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D264" s="39" t="str">
+        <f>'Test scenarios'!A262&amp;'Test scenarios'!B262</f>
+        <v/>
+      </c>
+    </row>
+    <row r="265" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D265" s="39" t="str">
+        <f>'Test scenarios'!A263&amp;'Test scenarios'!B263</f>
+        <v/>
+      </c>
+    </row>
+    <row r="266" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D266" s="39" t="str">
+        <f>'Test scenarios'!A264&amp;'Test scenarios'!B264</f>
+        <v/>
+      </c>
+    </row>
+    <row r="267" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D267" s="39" t="str">
+        <f>'Test scenarios'!A265&amp;'Test scenarios'!B265</f>
+        <v/>
+      </c>
+    </row>
+    <row r="268" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D268" s="39" t="str">
+        <f>'Test scenarios'!A266&amp;'Test scenarios'!B266</f>
+        <v/>
+      </c>
+    </row>
+    <row r="269" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D269" s="39" t="str">
+        <f>'Test scenarios'!A267&amp;'Test scenarios'!B267</f>
+        <v/>
+      </c>
+    </row>
+    <row r="270" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D270" s="39" t="str">
+        <f>'Test scenarios'!A268&amp;'Test scenarios'!B268</f>
+        <v/>
+      </c>
+    </row>
+    <row r="271" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D271" s="39" t="str">
+        <f>'Test scenarios'!A269&amp;'Test scenarios'!B269</f>
+        <v/>
+      </c>
+    </row>
+    <row r="272" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D272" s="39" t="str">
+        <f>'Test scenarios'!A270&amp;'Test scenarios'!B270</f>
+        <v/>
+      </c>
+    </row>
+    <row r="273" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D273" s="39" t="str">
+        <f>'Test scenarios'!A271&amp;'Test scenarios'!B271</f>
+        <v/>
+      </c>
+    </row>
+    <row r="274" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D274" s="39" t="str">
+        <f>'Test scenarios'!A272&amp;'Test scenarios'!B272</f>
+        <v/>
+      </c>
+    </row>
+    <row r="275" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D275" s="39" t="str">
+        <f>'Test scenarios'!A273&amp;'Test scenarios'!B273</f>
+        <v/>
+      </c>
+    </row>
+    <row r="276" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D276" s="39" t="str">
+        <f>'Test scenarios'!A274&amp;'Test scenarios'!B274</f>
+        <v/>
+      </c>
+    </row>
+    <row r="277" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D277" s="39" t="str">
+        <f>'Test scenarios'!A275&amp;'Test scenarios'!B275</f>
+        <v/>
+      </c>
+    </row>
+    <row r="278" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D278" s="39" t="str">
+        <f>'Test scenarios'!A276&amp;'Test scenarios'!B276</f>
+        <v/>
+      </c>
+    </row>
+    <row r="279" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D279" s="39" t="str">
+        <f>'Test scenarios'!A277&amp;'Test scenarios'!B277</f>
+        <v/>
+      </c>
+    </row>
+    <row r="280" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D280" s="39" t="str">
+        <f>'Test scenarios'!A278&amp;'Test scenarios'!B278</f>
+        <v/>
+      </c>
+    </row>
+    <row r="281" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D281" s="39" t="str">
+        <f>'Test scenarios'!A279&amp;'Test scenarios'!B279</f>
+        <v/>
+      </c>
+    </row>
+    <row r="282" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D282" s="39" t="str">
+        <f>'Test scenarios'!A280&amp;'Test scenarios'!B280</f>
+        <v/>
+      </c>
+    </row>
+    <row r="283" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D283" s="39" t="str">
+        <f>'Test scenarios'!A281&amp;'Test scenarios'!B281</f>
+        <v/>
+      </c>
+    </row>
+    <row r="284" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D284" s="39" t="str">
+        <f>'Test scenarios'!A282&amp;'Test scenarios'!B282</f>
+        <v/>
+      </c>
+    </row>
+    <row r="285" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D285" s="39" t="str">
+        <f>'Test scenarios'!A283&amp;'Test scenarios'!B283</f>
+        <v/>
+      </c>
+    </row>
+    <row r="286" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D286" s="39" t="str">
+        <f>'Test scenarios'!A284&amp;'Test scenarios'!B284</f>
+        <v/>
+      </c>
+    </row>
+    <row r="287" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D287" s="39" t="str">
+        <f>'Test scenarios'!A285&amp;'Test scenarios'!B285</f>
+        <v/>
+      </c>
+    </row>
+    <row r="288" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D288" s="39" t="str">
+        <f>'Test scenarios'!A286&amp;'Test scenarios'!B286</f>
+        <v/>
+      </c>
+    </row>
+    <row r="289" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D289" s="39" t="str">
+        <f>'Test scenarios'!A287&amp;'Test scenarios'!B287</f>
+        <v/>
+      </c>
+    </row>
+    <row r="290" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D290" s="39" t="str">
+        <f>'Test scenarios'!A288&amp;'Test scenarios'!B288</f>
+        <v/>
+      </c>
+    </row>
+    <row r="291" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D291" s="39" t="str">
+        <f>'Test scenarios'!A289&amp;'Test scenarios'!B289</f>
+        <v/>
+      </c>
+    </row>
+    <row r="292" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D292" s="39" t="str">
+        <f>'Test scenarios'!A290&amp;'Test scenarios'!B290</f>
+        <v/>
+      </c>
+    </row>
+    <row r="293" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D293" s="39" t="str">
+        <f>'Test scenarios'!A291&amp;'Test scenarios'!B291</f>
+        <v/>
+      </c>
+    </row>
+    <row r="294" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D294" s="39" t="str">
+        <f>'Test scenarios'!A292&amp;'Test scenarios'!B292</f>
+        <v/>
+      </c>
+    </row>
+    <row r="295" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D295" s="39" t="str">
+        <f>'Test scenarios'!A293&amp;'Test scenarios'!B293</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D296" s="39" t="str">
+        <f>'Test scenarios'!A294&amp;'Test scenarios'!B294</f>
+        <v/>
+      </c>
+    </row>
+    <row r="297" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D297" s="39" t="str">
+        <f>'Test scenarios'!A295&amp;'Test scenarios'!B295</f>
+        <v/>
+      </c>
+    </row>
+    <row r="298" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D298" s="39" t="str">
+        <f>'Test scenarios'!A296&amp;'Test scenarios'!B296</f>
+        <v/>
+      </c>
+    </row>
+    <row r="299" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D299" s="39" t="str">
+        <f>'Test scenarios'!A297&amp;'Test scenarios'!B297</f>
+        <v/>
+      </c>
+    </row>
+    <row r="300" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D300" s="39" t="str">
+        <f>'Test scenarios'!A298&amp;'Test scenarios'!B298</f>
+        <v/>
+      </c>
+    </row>
+    <row r="301" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D301" s="39" t="str">
+        <f>'Test scenarios'!A299&amp;'Test scenarios'!B299</f>
+        <v/>
+      </c>
+    </row>
+    <row r="302" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D302" s="39" t="str">
+        <f>'Test scenarios'!A300&amp;'Test scenarios'!B300</f>
+        <v/>
+      </c>
+    </row>
+    <row r="303" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D303" s="39" t="str">
+        <f>'Test scenarios'!A301&amp;'Test scenarios'!B301</f>
+        <v/>
+      </c>
+    </row>
+    <row r="304" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D304" s="39" t="str">
+        <f>'Test scenarios'!A302&amp;'Test scenarios'!B302</f>
+        <v/>
+      </c>
+    </row>
+    <row r="305" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D305" s="39" t="str">
+        <f>'Test scenarios'!A303&amp;'Test scenarios'!B303</f>
+        <v/>
+      </c>
+    </row>
+    <row r="306" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D306" s="39" t="str">
+        <f>'Test scenarios'!A304&amp;'Test scenarios'!B304</f>
+        <v/>
+      </c>
+    </row>
+    <row r="307" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D307" s="39" t="str">
+        <f>'Test scenarios'!A305&amp;'Test scenarios'!B305</f>
+        <v/>
+      </c>
+    </row>
+    <row r="308" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D308" s="39" t="str">
+        <f>'Test scenarios'!A306&amp;'Test scenarios'!B306</f>
+        <v/>
+      </c>
+    </row>
+    <row r="309" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D309" s="39" t="str">
+        <f>'Test scenarios'!A307&amp;'Test scenarios'!B307</f>
+        <v/>
+      </c>
+    </row>
+    <row r="310" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D310" s="39" t="str">
+        <f>'Test scenarios'!A308&amp;'Test scenarios'!B308</f>
+        <v/>
+      </c>
+    </row>
+    <row r="311" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D311" s="39" t="str">
+        <f>'Test scenarios'!A309&amp;'Test scenarios'!B309</f>
+        <v/>
+      </c>
+    </row>
+    <row r="312" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D312" s="39" t="str">
+        <f>'Test scenarios'!A310&amp;'Test scenarios'!B310</f>
+        <v/>
+      </c>
+    </row>
+    <row r="313" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D313" s="39" t="str">
+        <f>'Test scenarios'!A311&amp;'Test scenarios'!B311</f>
+        <v/>
+      </c>
+    </row>
+    <row r="314" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D314" s="39" t="str">
+        <f>'Test scenarios'!A312&amp;'Test scenarios'!B312</f>
+        <v/>
+      </c>
+    </row>
+    <row r="315" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D315" s="39" t="str">
+        <f>'Test scenarios'!A313&amp;'Test scenarios'!B313</f>
+        <v/>
+      </c>
+    </row>
+    <row r="316" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D316" s="39" t="str">
+        <f>'Test scenarios'!A314&amp;'Test scenarios'!B314</f>
+        <v/>
+      </c>
+    </row>
+    <row r="317" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D317" s="39" t="str">
+        <f>'Test scenarios'!A315&amp;'Test scenarios'!B315</f>
+        <v/>
+      </c>
+    </row>
+    <row r="318" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D318" s="39" t="str">
+        <f>'Test scenarios'!A316&amp;'Test scenarios'!B316</f>
+        <v/>
+      </c>
+    </row>
+    <row r="319" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D319" s="39" t="str">
+        <f>'Test scenarios'!A317&amp;'Test scenarios'!B317</f>
+        <v/>
+      </c>
+    </row>
+    <row r="320" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D320" s="39" t="str">
+        <f>'Test scenarios'!A318&amp;'Test scenarios'!B318</f>
+        <v/>
+      </c>
+    </row>
+    <row r="321" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D321" s="39" t="str">
+        <f>'Test scenarios'!A319&amp;'Test scenarios'!B319</f>
+        <v/>
+      </c>
+    </row>
+    <row r="322" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D322" s="39" t="str">
+        <f>'Test scenarios'!A320&amp;'Test scenarios'!B320</f>
+        <v/>
+      </c>
+    </row>
+    <row r="323" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D323" s="39" t="str">
+        <f>'Test scenarios'!A321&amp;'Test scenarios'!B321</f>
+        <v/>
+      </c>
+    </row>
+    <row r="324" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D324" s="39" t="str">
+        <f>'Test scenarios'!A322&amp;'Test scenarios'!B322</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>